<commit_message>
Correcciones de Supermercado dise;o generales, mobile y desktop
</commit_message>
<xml_diff>
--- a/Dietetica/1 Desarrollo/Recursos/MecohueDB.xlsx
+++ b/Dietetica/1 Desarrollo/Recursos/MecohueDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\RIMOARCHIVOS\Desktop\Rimo 2\Taller\PROYECTOS\WEB-MOBILE\BOTH\Independencia Monetaria\El Chango de Ale\1 Desarrollo\Dietetica\1 Desarrollo\Recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2481C6E4-7407-4852-B5CE-E192929118CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D61E70-E939-4EA7-BB15-26DA319EE4DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B0ADD01D-6BAD-4B76-86D2-01968970A8A0}"/>
   </bookViews>
@@ -3005,6 +3005,333 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="13" fillId="6" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="13" fillId="6" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="13" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="13" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="6" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3057,333 +3384,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="6" fontId="6" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="6" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="6" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="13" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="13" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="13" fillId="6" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="13" fillId="6" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3702,8 +3702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D192512-027D-4ECB-963C-63A3F8E96767}">
   <dimension ref="A1:H274"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A211" workbookViewId="0">
-      <selection activeCell="C125" sqref="C125:E125"/>
+    <sheetView tabSelected="1" topLeftCell="B236" workbookViewId="0">
+      <selection activeCell="L240" sqref="L240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3714,37 +3714,37 @@
       <c r="C1" s="3"/>
       <c r="D1" s="4"/>
       <c r="E1" s="5"/>
-      <c r="F1" s="66" t="s">
+      <c r="F1" s="175" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="67"/>
-      <c r="H1" s="68"/>
+      <c r="G1" s="176"/>
+      <c r="H1" s="177"/>
     </row>
     <row r="2" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="B2" s="7"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="72" t="s">
+      <c r="C2" s="178"/>
+      <c r="D2" s="179"/>
+      <c r="E2" s="180"/>
+      <c r="F2" s="181" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="73"/>
-      <c r="H2" s="74"/>
+      <c r="G2" s="182"/>
+      <c r="H2" s="183"/>
     </row>
     <row r="3" spans="1:8" ht="37.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8"/>
       <c r="B3" s="9"/>
-      <c r="C3" s="75" t="s">
+      <c r="C3" s="184" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="76"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="78" t="s">
+      <c r="D3" s="185"/>
+      <c r="E3" s="186"/>
+      <c r="F3" s="187" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="79"/>
-      <c r="H3" s="80"/>
+      <c r="G3" s="188"/>
+      <c r="H3" s="189"/>
     </row>
     <row r="4" spans="1:8" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
@@ -3758,25 +3758,25 @@
       <c r="E4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="81" t="s">
+      <c r="F4" s="190" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="82"/>
-      <c r="H4" s="83"/>
+      <c r="G4" s="191"/>
+      <c r="H4" s="192"/>
     </row>
     <row r="5" spans="1:8" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8"/>
       <c r="B5" s="9"/>
-      <c r="C5" s="84" t="s">
+      <c r="C5" s="169" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="85"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="87">
+      <c r="D5" s="170"/>
+      <c r="E5" s="171"/>
+      <c r="F5" s="172">
         <v>30000</v>
       </c>
-      <c r="G5" s="88"/>
-      <c r="H5" s="89"/>
+      <c r="G5" s="173"/>
+      <c r="H5" s="174"/>
     </row>
     <row r="6" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8"/>
@@ -3790,8 +3790,8 @@
       <c r="E6" s="14">
         <v>6330</v>
       </c>
-      <c r="F6" s="90"/>
-      <c r="G6" s="91"/>
+      <c r="F6" s="104"/>
+      <c r="G6" s="146"/>
       <c r="H6" s="15"/>
     </row>
     <row r="7" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3806,8 +3806,8 @@
       <c r="E7" s="14">
         <v>3320</v>
       </c>
-      <c r="F7" s="90"/>
-      <c r="G7" s="91"/>
+      <c r="F7" s="104"/>
+      <c r="G7" s="146"/>
       <c r="H7" s="15"/>
     </row>
     <row r="8" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3822,10 +3822,10 @@
       <c r="E8" s="14">
         <v>7450</v>
       </c>
-      <c r="F8" s="92" t="s">
+      <c r="F8" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="93"/>
+      <c r="G8" s="103"/>
       <c r="H8" s="15"/>
     </row>
     <row r="9" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3840,10 +3840,10 @@
       <c r="E9" s="14">
         <v>3780</v>
       </c>
-      <c r="F9" s="92" t="s">
+      <c r="F9" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="93"/>
+      <c r="G9" s="103"/>
       <c r="H9" s="15"/>
     </row>
     <row r="10" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3858,9 +3858,9 @@
       <c r="E10" s="14">
         <v>10260</v>
       </c>
-      <c r="F10" s="90"/>
-      <c r="G10" s="94"/>
-      <c r="H10" s="91"/>
+      <c r="F10" s="104"/>
+      <c r="G10" s="105"/>
+      <c r="H10" s="146"/>
     </row>
     <row r="11" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
@@ -3874,9 +3874,9 @@
       <c r="E11" s="14">
         <v>5160</v>
       </c>
-      <c r="F11" s="90"/>
-      <c r="G11" s="94"/>
-      <c r="H11" s="91"/>
+      <c r="F11" s="104"/>
+      <c r="G11" s="105"/>
+      <c r="H11" s="146"/>
     </row>
     <row r="12" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
@@ -3890,9 +3890,9 @@
       <c r="E12" s="14">
         <v>12970</v>
       </c>
-      <c r="F12" s="90"/>
-      <c r="G12" s="94"/>
-      <c r="H12" s="91"/>
+      <c r="F12" s="104"/>
+      <c r="G12" s="105"/>
+      <c r="H12" s="146"/>
     </row>
     <row r="13" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="16"/>
@@ -3906,9 +3906,9 @@
       <c r="E13" s="14">
         <v>6520</v>
       </c>
-      <c r="F13" s="90"/>
-      <c r="G13" s="94"/>
-      <c r="H13" s="91"/>
+      <c r="F13" s="104"/>
+      <c r="G13" s="105"/>
+      <c r="H13" s="146"/>
     </row>
     <row r="14" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
@@ -3922,9 +3922,9 @@
       <c r="E14" s="14">
         <v>6380</v>
       </c>
-      <c r="F14" s="90"/>
-      <c r="G14" s="94"/>
-      <c r="H14" s="91"/>
+      <c r="F14" s="104"/>
+      <c r="G14" s="105"/>
+      <c r="H14" s="146"/>
     </row>
     <row r="15" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
@@ -3938,9 +3938,9 @@
       <c r="E15" s="14">
         <v>3340</v>
       </c>
-      <c r="F15" s="90"/>
-      <c r="G15" s="94"/>
-      <c r="H15" s="91"/>
+      <c r="F15" s="104"/>
+      <c r="G15" s="105"/>
+      <c r="H15" s="146"/>
     </row>
     <row r="16" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16"/>
@@ -3954,9 +3954,9 @@
       <c r="E16" s="14">
         <v>3490</v>
       </c>
-      <c r="F16" s="90"/>
-      <c r="G16" s="94"/>
-      <c r="H16" s="91"/>
+      <c r="F16" s="104"/>
+      <c r="G16" s="105"/>
+      <c r="H16" s="146"/>
     </row>
     <row r="17" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16"/>
@@ -3970,9 +3970,9 @@
       <c r="E17" s="14">
         <v>2630</v>
       </c>
-      <c r="F17" s="90"/>
-      <c r="G17" s="94"/>
-      <c r="H17" s="91"/>
+      <c r="F17" s="104"/>
+      <c r="G17" s="105"/>
+      <c r="H17" s="146"/>
     </row>
     <row r="18" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16"/>
@@ -3986,9 +3986,9 @@
       <c r="E18" s="14">
         <v>12030</v>
       </c>
-      <c r="F18" s="90"/>
-      <c r="G18" s="94"/>
-      <c r="H18" s="91"/>
+      <c r="F18" s="104"/>
+      <c r="G18" s="105"/>
+      <c r="H18" s="146"/>
     </row>
     <row r="19" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="16"/>
@@ -4002,9 +4002,9 @@
       <c r="E19" s="14">
         <v>4230</v>
       </c>
-      <c r="F19" s="90"/>
-      <c r="G19" s="94"/>
-      <c r="H19" s="91"/>
+      <c r="F19" s="104"/>
+      <c r="G19" s="105"/>
+      <c r="H19" s="146"/>
     </row>
     <row r="20" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="16"/>
@@ -4018,9 +4018,9 @@
       <c r="E20" s="14">
         <v>4310</v>
       </c>
-      <c r="F20" s="90"/>
-      <c r="G20" s="94"/>
-      <c r="H20" s="91"/>
+      <c r="F20" s="104"/>
+      <c r="G20" s="105"/>
+      <c r="H20" s="146"/>
     </row>
     <row r="21" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16"/>
@@ -4034,9 +4034,9 @@
       <c r="E21" s="14">
         <v>10760</v>
       </c>
-      <c r="F21" s="90"/>
-      <c r="G21" s="94"/>
-      <c r="H21" s="91"/>
+      <c r="F21" s="104"/>
+      <c r="G21" s="105"/>
+      <c r="H21" s="146"/>
     </row>
     <row r="22" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="16"/>
@@ -4050,9 +4050,9 @@
       <c r="E22" s="14">
         <v>4140</v>
       </c>
-      <c r="F22" s="90"/>
-      <c r="G22" s="94"/>
-      <c r="H22" s="91"/>
+      <c r="F22" s="104"/>
+      <c r="G22" s="105"/>
+      <c r="H22" s="146"/>
     </row>
     <row r="23" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="16"/>
@@ -4066,9 +4066,9 @@
       <c r="E23" s="14">
         <v>3060</v>
       </c>
-      <c r="F23" s="90"/>
-      <c r="G23" s="94"/>
-      <c r="H23" s="91"/>
+      <c r="F23" s="104"/>
+      <c r="G23" s="105"/>
+      <c r="H23" s="146"/>
     </row>
     <row r="24" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="16"/>
@@ -4082,21 +4082,21 @@
       <c r="E24" s="21">
         <v>6000</v>
       </c>
-      <c r="F24" s="90"/>
-      <c r="G24" s="94"/>
-      <c r="H24" s="91"/>
+      <c r="F24" s="104"/>
+      <c r="G24" s="105"/>
+      <c r="H24" s="146"/>
     </row>
     <row r="25" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="8"/>
       <c r="B25" s="9"/>
-      <c r="C25" s="95" t="s">
+      <c r="C25" s="166" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="96"/>
-      <c r="E25" s="97"/>
-      <c r="F25" s="98"/>
-      <c r="G25" s="94"/>
-      <c r="H25" s="91"/>
+      <c r="D25" s="167"/>
+      <c r="E25" s="168"/>
+      <c r="F25" s="119"/>
+      <c r="G25" s="105"/>
+      <c r="H25" s="146"/>
     </row>
     <row r="26" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="16"/>
@@ -4110,9 +4110,9 @@
       <c r="E26" s="14">
         <v>8030</v>
       </c>
-      <c r="F26" s="90"/>
-      <c r="G26" s="94"/>
-      <c r="H26" s="91"/>
+      <c r="F26" s="104"/>
+      <c r="G26" s="105"/>
+      <c r="H26" s="146"/>
     </row>
     <row r="27" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="16"/>
@@ -4126,9 +4126,9 @@
       <c r="E27" s="14">
         <v>15750</v>
       </c>
-      <c r="F27" s="90"/>
-      <c r="G27" s="94"/>
-      <c r="H27" s="91"/>
+      <c r="F27" s="104"/>
+      <c r="G27" s="105"/>
+      <c r="H27" s="146"/>
     </row>
     <row r="28" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="16"/>
@@ -4142,9 +4142,9 @@
       <c r="E28" s="14">
         <v>7650</v>
       </c>
-      <c r="F28" s="90"/>
-      <c r="G28" s="94"/>
-      <c r="H28" s="91"/>
+      <c r="F28" s="104"/>
+      <c r="G28" s="105"/>
+      <c r="H28" s="146"/>
     </row>
     <row r="29" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="16"/>
@@ -4158,9 +4158,9 @@
       <c r="E29" s="14">
         <v>15000</v>
       </c>
-      <c r="F29" s="90"/>
-      <c r="G29" s="94"/>
-      <c r="H29" s="91"/>
+      <c r="F29" s="104"/>
+      <c r="G29" s="105"/>
+      <c r="H29" s="146"/>
     </row>
     <row r="30" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="16"/>
@@ -4174,9 +4174,9 @@
       <c r="E30" s="14">
         <v>10650</v>
       </c>
-      <c r="F30" s="90"/>
-      <c r="G30" s="94"/>
-      <c r="H30" s="91"/>
+      <c r="F30" s="104"/>
+      <c r="G30" s="105"/>
+      <c r="H30" s="146"/>
     </row>
     <row r="31" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="16"/>
@@ -4190,9 +4190,9 @@
       <c r="E31" s="14">
         <v>4130</v>
       </c>
-      <c r="F31" s="90"/>
-      <c r="G31" s="94"/>
-      <c r="H31" s="91"/>
+      <c r="F31" s="104"/>
+      <c r="G31" s="105"/>
+      <c r="H31" s="146"/>
     </row>
     <row r="32" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="16"/>
@@ -4206,9 +4206,9 @@
       <c r="E32" s="14">
         <v>7950</v>
       </c>
-      <c r="F32" s="90"/>
-      <c r="G32" s="94"/>
-      <c r="H32" s="91"/>
+      <c r="F32" s="104"/>
+      <c r="G32" s="105"/>
+      <c r="H32" s="146"/>
     </row>
     <row r="33" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="16"/>
@@ -4222,9 +4222,9 @@
       <c r="E33" s="14">
         <v>17220</v>
       </c>
-      <c r="F33" s="90"/>
-      <c r="G33" s="94"/>
-      <c r="H33" s="91"/>
+      <c r="F33" s="104"/>
+      <c r="G33" s="105"/>
+      <c r="H33" s="146"/>
     </row>
     <row r="34" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="16"/>
@@ -4238,9 +4238,9 @@
       <c r="E34" s="14">
         <v>34130</v>
       </c>
-      <c r="F34" s="90"/>
-      <c r="G34" s="94"/>
-      <c r="H34" s="91"/>
+      <c r="F34" s="104"/>
+      <c r="G34" s="105"/>
+      <c r="H34" s="146"/>
     </row>
     <row r="35" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="16"/>
@@ -4254,9 +4254,9 @@
       <c r="E35" s="14">
         <v>11480</v>
       </c>
-      <c r="F35" s="90"/>
-      <c r="G35" s="94"/>
-      <c r="H35" s="91"/>
+      <c r="F35" s="104"/>
+      <c r="G35" s="105"/>
+      <c r="H35" s="146"/>
     </row>
     <row r="36" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="16"/>
@@ -4270,9 +4270,9 @@
       <c r="E36" s="14">
         <v>22650</v>
       </c>
-      <c r="F36" s="90"/>
-      <c r="G36" s="94"/>
-      <c r="H36" s="91"/>
+      <c r="F36" s="104"/>
+      <c r="G36" s="105"/>
+      <c r="H36" s="146"/>
     </row>
     <row r="37" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="16"/>
@@ -4286,9 +4286,9 @@
       <c r="E37" s="14">
         <v>10280</v>
       </c>
-      <c r="F37" s="90"/>
-      <c r="G37" s="94"/>
-      <c r="H37" s="91"/>
+      <c r="F37" s="104"/>
+      <c r="G37" s="105"/>
+      <c r="H37" s="146"/>
     </row>
     <row r="38" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="16"/>
@@ -4302,9 +4302,9 @@
       <c r="E38" s="14">
         <v>20250</v>
       </c>
-      <c r="F38" s="90"/>
-      <c r="G38" s="94"/>
-      <c r="H38" s="91"/>
+      <c r="F38" s="104"/>
+      <c r="G38" s="105"/>
+      <c r="H38" s="146"/>
     </row>
     <row r="39" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="16"/>
@@ -4318,9 +4318,9 @@
       <c r="E39" s="14">
         <v>13730</v>
       </c>
-      <c r="F39" s="90"/>
-      <c r="G39" s="94"/>
-      <c r="H39" s="91"/>
+      <c r="F39" s="104"/>
+      <c r="G39" s="105"/>
+      <c r="H39" s="146"/>
     </row>
     <row r="40" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="16"/>
@@ -4334,9 +4334,9 @@
       <c r="E40" s="14">
         <v>27150</v>
       </c>
-      <c r="F40" s="90"/>
-      <c r="G40" s="94"/>
-      <c r="H40" s="91"/>
+      <c r="F40" s="104"/>
+      <c r="G40" s="105"/>
+      <c r="H40" s="146"/>
     </row>
     <row r="41" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="16"/>
@@ -4350,9 +4350,9 @@
       <c r="E41" s="14">
         <v>8420</v>
       </c>
-      <c r="F41" s="90"/>
-      <c r="G41" s="94"/>
-      <c r="H41" s="91"/>
+      <c r="F41" s="104"/>
+      <c r="G41" s="105"/>
+      <c r="H41" s="146"/>
     </row>
     <row r="42" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="8"/>
@@ -4366,10 +4366,10 @@
       <c r="E42" s="14">
         <v>14500</v>
       </c>
-      <c r="F42" s="92" t="s">
+      <c r="F42" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="G42" s="93"/>
+      <c r="G42" s="103"/>
       <c r="H42" s="15"/>
     </row>
     <row r="43" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4384,9 +4384,9 @@
       <c r="E43" s="14">
         <v>9120</v>
       </c>
-      <c r="F43" s="90"/>
-      <c r="G43" s="94"/>
-      <c r="H43" s="91"/>
+      <c r="F43" s="104"/>
+      <c r="G43" s="105"/>
+      <c r="H43" s="146"/>
     </row>
     <row r="44" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="8"/>
@@ -4400,9 +4400,9 @@
       <c r="E44" s="14">
         <v>17940</v>
       </c>
-      <c r="F44" s="90"/>
-      <c r="G44" s="94"/>
-      <c r="H44" s="91"/>
+      <c r="F44" s="104"/>
+      <c r="G44" s="105"/>
+      <c r="H44" s="146"/>
     </row>
     <row r="45" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="8"/>
@@ -4416,21 +4416,21 @@
       <c r="E45" s="26">
         <v>5410</v>
       </c>
-      <c r="F45" s="99"/>
-      <c r="G45" s="94"/>
-      <c r="H45" s="91"/>
+      <c r="F45" s="115"/>
+      <c r="G45" s="105"/>
+      <c r="H45" s="146"/>
     </row>
     <row r="46" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="8"/>
       <c r="B46" s="9"/>
-      <c r="C46" s="100" t="s">
+      <c r="C46" s="163" t="s">
         <v>44</v>
       </c>
-      <c r="D46" s="101"/>
-      <c r="E46" s="102"/>
-      <c r="F46" s="98"/>
-      <c r="G46" s="94"/>
-      <c r="H46" s="91"/>
+      <c r="D46" s="164"/>
+      <c r="E46" s="165"/>
+      <c r="F46" s="119"/>
+      <c r="G46" s="105"/>
+      <c r="H46" s="146"/>
     </row>
     <row r="47" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="8"/>
@@ -4444,9 +4444,9 @@
       <c r="E47" s="14">
         <v>2500</v>
       </c>
-      <c r="F47" s="90"/>
-      <c r="G47" s="94"/>
-      <c r="H47" s="91"/>
+      <c r="F47" s="104"/>
+      <c r="G47" s="105"/>
+      <c r="H47" s="146"/>
     </row>
     <row r="48" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="16"/>
@@ -4460,9 +4460,9 @@
       <c r="E48" s="14">
         <v>6300</v>
       </c>
-      <c r="F48" s="90"/>
-      <c r="G48" s="94"/>
-      <c r="H48" s="91"/>
+      <c r="F48" s="104"/>
+      <c r="G48" s="105"/>
+      <c r="H48" s="146"/>
     </row>
     <row r="49" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="16"/>
@@ -4476,9 +4476,9 @@
       <c r="E49" s="14">
         <v>6950</v>
       </c>
-      <c r="F49" s="90"/>
-      <c r="G49" s="94"/>
-      <c r="H49" s="91"/>
+      <c r="F49" s="104"/>
+      <c r="G49" s="105"/>
+      <c r="H49" s="146"/>
     </row>
     <row r="50" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="16"/>
@@ -4492,9 +4492,9 @@
       <c r="E50" s="14">
         <v>4720</v>
       </c>
-      <c r="F50" s="90"/>
-      <c r="G50" s="94"/>
-      <c r="H50" s="91"/>
+      <c r="F50" s="104"/>
+      <c r="G50" s="105"/>
+      <c r="H50" s="146"/>
     </row>
     <row r="51" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="16"/>
@@ -4508,9 +4508,9 @@
       <c r="E51" s="14">
         <v>1460</v>
       </c>
-      <c r="F51" s="90"/>
-      <c r="G51" s="94"/>
-      <c r="H51" s="91"/>
+      <c r="F51" s="104"/>
+      <c r="G51" s="105"/>
+      <c r="H51" s="146"/>
     </row>
     <row r="52" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="16"/>
@@ -4524,9 +4524,9 @@
       <c r="E52" s="14">
         <v>2630</v>
       </c>
-      <c r="F52" s="90"/>
-      <c r="G52" s="94"/>
-      <c r="H52" s="91"/>
+      <c r="F52" s="104"/>
+      <c r="G52" s="105"/>
+      <c r="H52" s="146"/>
     </row>
     <row r="53" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="16"/>
@@ -4540,9 +4540,9 @@
       <c r="E53" s="14">
         <v>2100</v>
       </c>
-      <c r="F53" s="90"/>
-      <c r="G53" s="94"/>
-      <c r="H53" s="91"/>
+      <c r="F53" s="104"/>
+      <c r="G53" s="105"/>
+      <c r="H53" s="146"/>
     </row>
     <row r="54" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="16"/>
@@ -4556,9 +4556,9 @@
       <c r="E54" s="14">
         <v>3900</v>
       </c>
-      <c r="F54" s="90"/>
-      <c r="G54" s="94"/>
-      <c r="H54" s="91"/>
+      <c r="F54" s="104"/>
+      <c r="G54" s="105"/>
+      <c r="H54" s="146"/>
     </row>
     <row r="55" spans="1:8" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="16"/>
@@ -4572,9 +4572,9 @@
       <c r="E55" s="14">
         <v>7800</v>
       </c>
-      <c r="F55" s="90"/>
-      <c r="G55" s="94"/>
-      <c r="H55" s="91"/>
+      <c r="F55" s="104"/>
+      <c r="G55" s="105"/>
+      <c r="H55" s="146"/>
     </row>
     <row r="56" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="16"/>
@@ -4588,9 +4588,9 @@
       <c r="E56" s="14">
         <v>6300</v>
       </c>
-      <c r="F56" s="90"/>
-      <c r="G56" s="94"/>
-      <c r="H56" s="91"/>
+      <c r="F56" s="104"/>
+      <c r="G56" s="105"/>
+      <c r="H56" s="146"/>
     </row>
     <row r="57" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="16"/>
@@ -4604,9 +4604,9 @@
       <c r="E57" s="14">
         <v>7200</v>
       </c>
-      <c r="F57" s="90"/>
-      <c r="G57" s="94"/>
-      <c r="H57" s="91"/>
+      <c r="F57" s="104"/>
+      <c r="G57" s="105"/>
+      <c r="H57" s="146"/>
     </row>
     <row r="58" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="16"/>
@@ -4620,10 +4620,10 @@
       <c r="E58" s="14">
         <v>5150</v>
       </c>
-      <c r="F58" s="92" t="s">
+      <c r="F58" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="G58" s="93"/>
+      <c r="G58" s="103"/>
       <c r="H58" s="15"/>
     </row>
     <row r="59" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4638,9 +4638,9 @@
       <c r="E59" s="14">
         <v>7490</v>
       </c>
-      <c r="F59" s="90"/>
-      <c r="G59" s="94"/>
-      <c r="H59" s="91"/>
+      <c r="F59" s="104"/>
+      <c r="G59" s="105"/>
+      <c r="H59" s="146"/>
     </row>
     <row r="60" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="16"/>
@@ -4654,9 +4654,9 @@
       <c r="E60" s="14">
         <v>3900</v>
       </c>
-      <c r="F60" s="90"/>
-      <c r="G60" s="94"/>
-      <c r="H60" s="91"/>
+      <c r="F60" s="104"/>
+      <c r="G60" s="105"/>
+      <c r="H60" s="146"/>
     </row>
     <row r="61" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="16"/>
@@ -4670,9 +4670,9 @@
       <c r="E61" s="14">
         <v>12120</v>
       </c>
-      <c r="F61" s="90"/>
-      <c r="G61" s="94"/>
-      <c r="H61" s="91"/>
+      <c r="F61" s="104"/>
+      <c r="G61" s="105"/>
+      <c r="H61" s="146"/>
     </row>
     <row r="62" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="16"/>
@@ -4686,9 +4686,9 @@
       <c r="E62" s="14">
         <v>6210</v>
       </c>
-      <c r="F62" s="90"/>
-      <c r="G62" s="94"/>
-      <c r="H62" s="91"/>
+      <c r="F62" s="104"/>
+      <c r="G62" s="105"/>
+      <c r="H62" s="146"/>
     </row>
     <row r="63" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="16"/>
@@ -4702,9 +4702,9 @@
       <c r="E63" s="14">
         <v>12340</v>
       </c>
-      <c r="F63" s="90"/>
-      <c r="G63" s="94"/>
-      <c r="H63" s="91"/>
+      <c r="F63" s="104"/>
+      <c r="G63" s="105"/>
+      <c r="H63" s="146"/>
     </row>
     <row r="64" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="16"/>
@@ -4718,9 +4718,9 @@
       <c r="E64" s="14">
         <v>6320</v>
       </c>
-      <c r="F64" s="90"/>
-      <c r="G64" s="94"/>
-      <c r="H64" s="91"/>
+      <c r="F64" s="104"/>
+      <c r="G64" s="105"/>
+      <c r="H64" s="146"/>
     </row>
     <row r="65" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="16"/>
@@ -4734,9 +4734,9 @@
       <c r="E65" s="14">
         <v>9060</v>
       </c>
-      <c r="F65" s="90"/>
-      <c r="G65" s="94"/>
-      <c r="H65" s="91"/>
+      <c r="F65" s="104"/>
+      <c r="G65" s="105"/>
+      <c r="H65" s="146"/>
     </row>
     <row r="66" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="16"/>
@@ -4750,9 +4750,9 @@
       <c r="E66" s="14">
         <v>17810</v>
       </c>
-      <c r="F66" s="90"/>
-      <c r="G66" s="94"/>
-      <c r="H66" s="91"/>
+      <c r="F66" s="104"/>
+      <c r="G66" s="105"/>
+      <c r="H66" s="146"/>
     </row>
     <row r="67" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="16"/>
@@ -4766,9 +4766,9 @@
       <c r="E67" s="14">
         <v>11750</v>
       </c>
-      <c r="F67" s="90"/>
-      <c r="G67" s="94"/>
-      <c r="H67" s="91"/>
+      <c r="F67" s="104"/>
+      <c r="G67" s="105"/>
+      <c r="H67" s="146"/>
     </row>
     <row r="68" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="16"/>
@@ -4782,9 +4782,9 @@
       <c r="E68" s="14">
         <v>10010</v>
       </c>
-      <c r="F68" s="90"/>
-      <c r="G68" s="94"/>
-      <c r="H68" s="91"/>
+      <c r="F68" s="104"/>
+      <c r="G68" s="105"/>
+      <c r="H68" s="146"/>
     </row>
     <row r="69" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="16"/>
@@ -4798,9 +4798,9 @@
       <c r="E69" s="14">
         <v>12000</v>
       </c>
-      <c r="F69" s="90"/>
-      <c r="G69" s="94"/>
-      <c r="H69" s="91"/>
+      <c r="F69" s="104"/>
+      <c r="G69" s="105"/>
+      <c r="H69" s="146"/>
     </row>
     <row r="70" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="16"/>
@@ -4814,9 +4814,9 @@
       <c r="E70" s="14">
         <v>6150</v>
       </c>
-      <c r="F70" s="90"/>
-      <c r="G70" s="94"/>
-      <c r="H70" s="91"/>
+      <c r="F70" s="104"/>
+      <c r="G70" s="105"/>
+      <c r="H70" s="146"/>
     </row>
     <row r="71" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="16"/>
@@ -4830,8 +4830,8 @@
       <c r="E71" s="14">
         <v>18980</v>
       </c>
-      <c r="F71" s="90"/>
-      <c r="G71" s="91"/>
+      <c r="F71" s="104"/>
+      <c r="G71" s="146"/>
       <c r="H71" s="15"/>
     </row>
     <row r="72" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4846,9 +4846,9 @@
       <c r="E72" s="14">
         <v>9640</v>
       </c>
-      <c r="F72" s="90"/>
-      <c r="G72" s="94"/>
-      <c r="H72" s="91"/>
+      <c r="F72" s="104"/>
+      <c r="G72" s="105"/>
+      <c r="H72" s="146"/>
     </row>
     <row r="73" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="16"/>
@@ -4862,9 +4862,9 @@
       <c r="E73" s="14">
         <v>6320</v>
       </c>
-      <c r="F73" s="90"/>
-      <c r="G73" s="94"/>
-      <c r="H73" s="91"/>
+      <c r="F73" s="104"/>
+      <c r="G73" s="105"/>
+      <c r="H73" s="146"/>
     </row>
     <row r="74" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="16"/>
@@ -4878,9 +4878,9 @@
       <c r="E74" s="14">
         <v>7430</v>
       </c>
-      <c r="F74" s="90"/>
-      <c r="G74" s="94"/>
-      <c r="H74" s="91"/>
+      <c r="F74" s="104"/>
+      <c r="G74" s="105"/>
+      <c r="H74" s="146"/>
     </row>
     <row r="75" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="16"/>
@@ -4894,9 +4894,9 @@
       <c r="E75" s="14">
         <v>6670</v>
       </c>
-      <c r="F75" s="90"/>
-      <c r="G75" s="94"/>
-      <c r="H75" s="91"/>
+      <c r="F75" s="104"/>
+      <c r="G75" s="105"/>
+      <c r="H75" s="146"/>
     </row>
     <row r="76" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="16"/>
@@ -4910,9 +4910,9 @@
       <c r="E76" s="14">
         <v>7740</v>
       </c>
-      <c r="F76" s="90"/>
-      <c r="G76" s="94"/>
-      <c r="H76" s="91"/>
+      <c r="F76" s="104"/>
+      <c r="G76" s="105"/>
+      <c r="H76" s="146"/>
     </row>
     <row r="77" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="16"/>
@@ -4926,9 +4926,9 @@
       <c r="E77" s="14">
         <v>10040</v>
       </c>
-      <c r="F77" s="90"/>
-      <c r="G77" s="94"/>
-      <c r="H77" s="91"/>
+      <c r="F77" s="104"/>
+      <c r="G77" s="105"/>
+      <c r="H77" s="146"/>
     </row>
     <row r="78" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="16"/>
@@ -4942,9 +4942,9 @@
       <c r="E78" s="14">
         <v>5170</v>
       </c>
-      <c r="F78" s="90"/>
-      <c r="G78" s="94"/>
-      <c r="H78" s="91"/>
+      <c r="F78" s="104"/>
+      <c r="G78" s="105"/>
+      <c r="H78" s="146"/>
     </row>
     <row r="79" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="16"/>
@@ -4958,9 +4958,9 @@
       <c r="E79" s="14">
         <v>15530</v>
       </c>
-      <c r="F79" s="90"/>
-      <c r="G79" s="94"/>
-      <c r="H79" s="91"/>
+      <c r="F79" s="104"/>
+      <c r="G79" s="105"/>
+      <c r="H79" s="146"/>
     </row>
     <row r="80" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="8"/>
@@ -4974,9 +4974,9 @@
       <c r="E80" s="14">
         <v>7920</v>
       </c>
-      <c r="F80" s="90"/>
-      <c r="G80" s="94"/>
-      <c r="H80" s="91"/>
+      <c r="F80" s="104"/>
+      <c r="G80" s="105"/>
+      <c r="H80" s="146"/>
     </row>
     <row r="81" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="8"/>
@@ -4990,9 +4990,9 @@
       <c r="E81" s="14">
         <v>10300</v>
       </c>
-      <c r="F81" s="90"/>
-      <c r="G81" s="94"/>
-      <c r="H81" s="91"/>
+      <c r="F81" s="104"/>
+      <c r="G81" s="105"/>
+      <c r="H81" s="146"/>
     </row>
     <row r="82" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="8"/>
@@ -5006,9 +5006,9 @@
       <c r="E82" s="14">
         <v>8460</v>
       </c>
-      <c r="F82" s="90"/>
-      <c r="G82" s="94"/>
-      <c r="H82" s="91"/>
+      <c r="F82" s="104"/>
+      <c r="G82" s="105"/>
+      <c r="H82" s="146"/>
     </row>
     <row r="83" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="8"/>
@@ -5022,21 +5022,21 @@
       <c r="E83" s="21">
         <v>5140</v>
       </c>
-      <c r="F83" s="90"/>
-      <c r="G83" s="94"/>
-      <c r="H83" s="91"/>
+      <c r="F83" s="104"/>
+      <c r="G83" s="105"/>
+      <c r="H83" s="146"/>
     </row>
     <row r="84" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="8"/>
       <c r="B84" s="9"/>
-      <c r="C84" s="103" t="s">
+      <c r="C84" s="160" t="s">
         <v>75</v>
       </c>
-      <c r="D84" s="104"/>
-      <c r="E84" s="105"/>
-      <c r="F84" s="98"/>
-      <c r="G84" s="94"/>
-      <c r="H84" s="91"/>
+      <c r="D84" s="161"/>
+      <c r="E84" s="162"/>
+      <c r="F84" s="119"/>
+      <c r="G84" s="105"/>
+      <c r="H84" s="146"/>
     </row>
     <row r="85" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="8"/>
@@ -5050,8 +5050,8 @@
       <c r="E85" s="30">
         <v>5180</v>
       </c>
-      <c r="F85" s="90"/>
-      <c r="G85" s="91"/>
+      <c r="F85" s="104"/>
+      <c r="G85" s="146"/>
       <c r="H85" s="15"/>
     </row>
     <row r="86" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5066,9 +5066,9 @@
       <c r="E86" s="14">
         <v>2520</v>
       </c>
-      <c r="F86" s="90"/>
-      <c r="G86" s="94"/>
-      <c r="H86" s="91"/>
+      <c r="F86" s="104"/>
+      <c r="G86" s="105"/>
+      <c r="H86" s="146"/>
     </row>
     <row r="87" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="16"/>
@@ -5082,9 +5082,9 @@
       <c r="E87" s="14">
         <v>2600</v>
       </c>
-      <c r="F87" s="90"/>
-      <c r="G87" s="94"/>
-      <c r="H87" s="91"/>
+      <c r="F87" s="104"/>
+      <c r="G87" s="105"/>
+      <c r="H87" s="146"/>
     </row>
     <row r="88" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="16"/>
@@ -5098,9 +5098,9 @@
       <c r="E88" s="14">
         <v>2600</v>
       </c>
-      <c r="F88" s="90"/>
-      <c r="G88" s="94"/>
-      <c r="H88" s="91"/>
+      <c r="F88" s="104"/>
+      <c r="G88" s="105"/>
+      <c r="H88" s="146"/>
     </row>
     <row r="89" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="16"/>
@@ -5114,9 +5114,9 @@
       <c r="E89" s="14">
         <v>2600</v>
       </c>
-      <c r="F89" s="90"/>
-      <c r="G89" s="94"/>
-      <c r="H89" s="91"/>
+      <c r="F89" s="104"/>
+      <c r="G89" s="105"/>
+      <c r="H89" s="146"/>
     </row>
     <row r="90" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="16"/>
@@ -5130,8 +5130,8 @@
       <c r="E90" s="31">
         <v>3750</v>
       </c>
-      <c r="F90" s="106"/>
-      <c r="G90" s="91"/>
+      <c r="F90" s="150"/>
+      <c r="G90" s="146"/>
       <c r="H90" s="15"/>
     </row>
     <row r="91" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5146,8 +5146,8 @@
       <c r="E91" s="31">
         <v>4050</v>
       </c>
-      <c r="F91" s="106"/>
-      <c r="G91" s="91"/>
+      <c r="F91" s="150"/>
+      <c r="G91" s="146"/>
       <c r="H91" s="15"/>
     </row>
     <row r="92" spans="1:8" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5162,9 +5162,9 @@
       <c r="E92" s="31">
         <v>5970</v>
       </c>
-      <c r="F92" s="106"/>
-      <c r="G92" s="94"/>
-      <c r="H92" s="91"/>
+      <c r="F92" s="150"/>
+      <c r="G92" s="105"/>
+      <c r="H92" s="146"/>
     </row>
     <row r="93" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="16"/>
@@ -5178,9 +5178,9 @@
       <c r="E93" s="31">
         <v>1650</v>
       </c>
-      <c r="F93" s="106"/>
-      <c r="G93" s="94"/>
-      <c r="H93" s="91"/>
+      <c r="F93" s="150"/>
+      <c r="G93" s="105"/>
+      <c r="H93" s="146"/>
     </row>
     <row r="94" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="16"/>
@@ -5194,9 +5194,9 @@
       <c r="E94" s="31">
         <v>1810</v>
       </c>
-      <c r="F94" s="106"/>
-      <c r="G94" s="94"/>
-      <c r="H94" s="91"/>
+      <c r="F94" s="150"/>
+      <c r="G94" s="105"/>
+      <c r="H94" s="146"/>
     </row>
     <row r="95" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="16"/>
@@ -5210,8 +5210,8 @@
       <c r="E95" s="32">
         <v>1610</v>
       </c>
-      <c r="F95" s="106"/>
-      <c r="G95" s="91"/>
+      <c r="F95" s="150"/>
+      <c r="G95" s="146"/>
       <c r="H95" s="15"/>
     </row>
     <row r="96" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5226,8 +5226,8 @@
       <c r="E96" s="32">
         <v>1610</v>
       </c>
-      <c r="F96" s="106"/>
-      <c r="G96" s="91"/>
+      <c r="F96" s="150"/>
+      <c r="G96" s="146"/>
       <c r="H96" s="15"/>
     </row>
     <row r="97" spans="1:8" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5242,9 +5242,9 @@
       <c r="E97" s="35">
         <v>1800</v>
       </c>
-      <c r="F97" s="106"/>
-      <c r="G97" s="94"/>
-      <c r="H97" s="91"/>
+      <c r="F97" s="150"/>
+      <c r="G97" s="105"/>
+      <c r="H97" s="146"/>
     </row>
     <row r="98" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="16"/>
@@ -5258,8 +5258,8 @@
       <c r="E98" s="35">
         <v>1100</v>
       </c>
-      <c r="F98" s="106"/>
-      <c r="G98" s="91"/>
+      <c r="F98" s="150"/>
+      <c r="G98" s="146"/>
       <c r="H98" s="15"/>
     </row>
     <row r="99" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5274,9 +5274,9 @@
       <c r="E99" s="35">
         <v>1100</v>
       </c>
-      <c r="F99" s="106"/>
-      <c r="G99" s="94"/>
-      <c r="H99" s="91"/>
+      <c r="F99" s="150"/>
+      <c r="G99" s="105"/>
+      <c r="H99" s="146"/>
     </row>
     <row r="100" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="16"/>
@@ -5290,9 +5290,9 @@
       <c r="E100" s="35">
         <v>1390</v>
       </c>
-      <c r="F100" s="106"/>
-      <c r="G100" s="94"/>
-      <c r="H100" s="91"/>
+      <c r="F100" s="150"/>
+      <c r="G100" s="105"/>
+      <c r="H100" s="146"/>
     </row>
     <row r="101" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="16"/>
@@ -5306,9 +5306,9 @@
       <c r="E101" s="32">
         <v>1770</v>
       </c>
-      <c r="F101" s="106"/>
-      <c r="G101" s="94"/>
-      <c r="H101" s="91"/>
+      <c r="F101" s="150"/>
+      <c r="G101" s="105"/>
+      <c r="H101" s="146"/>
     </row>
     <row r="102" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="16"/>
@@ -5322,9 +5322,9 @@
       <c r="E102" s="32">
         <v>1260</v>
       </c>
-      <c r="F102" s="106"/>
-      <c r="G102" s="94"/>
-      <c r="H102" s="91"/>
+      <c r="F102" s="150"/>
+      <c r="G102" s="105"/>
+      <c r="H102" s="146"/>
     </row>
     <row r="103" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="16"/>
@@ -5338,9 +5338,9 @@
       <c r="E103" s="32">
         <v>1980</v>
       </c>
-      <c r="F103" s="106"/>
-      <c r="G103" s="94"/>
-      <c r="H103" s="91"/>
+      <c r="F103" s="150"/>
+      <c r="G103" s="105"/>
+      <c r="H103" s="146"/>
     </row>
     <row r="104" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="16"/>
@@ -5354,9 +5354,9 @@
       <c r="E104" s="32">
         <v>3190</v>
       </c>
-      <c r="F104" s="106"/>
-      <c r="G104" s="94"/>
-      <c r="H104" s="91"/>
+      <c r="F104" s="150"/>
+      <c r="G104" s="105"/>
+      <c r="H104" s="146"/>
     </row>
     <row r="105" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="16"/>
@@ -5370,9 +5370,9 @@
       <c r="E105" s="31">
         <v>3190</v>
       </c>
-      <c r="F105" s="106"/>
-      <c r="G105" s="94"/>
-      <c r="H105" s="91"/>
+      <c r="F105" s="150"/>
+      <c r="G105" s="105"/>
+      <c r="H105" s="146"/>
     </row>
     <row r="106" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="16"/>
@@ -5386,9 +5386,9 @@
       <c r="E106" s="31">
         <v>1640</v>
       </c>
-      <c r="F106" s="106"/>
-      <c r="G106" s="94"/>
-      <c r="H106" s="91"/>
+      <c r="F106" s="150"/>
+      <c r="G106" s="105"/>
+      <c r="H106" s="146"/>
     </row>
     <row r="107" spans="1:8" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="16"/>
@@ -5402,9 +5402,9 @@
       <c r="E107" s="32">
         <v>1370</v>
       </c>
-      <c r="F107" s="106"/>
-      <c r="G107" s="94"/>
-      <c r="H107" s="91"/>
+      <c r="F107" s="150"/>
+      <c r="G107" s="105"/>
+      <c r="H107" s="146"/>
     </row>
     <row r="108" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="16"/>
@@ -5418,9 +5418,9 @@
       <c r="E108" s="32">
         <v>1370</v>
       </c>
-      <c r="F108" s="106"/>
-      <c r="G108" s="94"/>
-      <c r="H108" s="91"/>
+      <c r="F108" s="150"/>
+      <c r="G108" s="105"/>
+      <c r="H108" s="146"/>
     </row>
     <row r="109" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="16"/>
@@ -5434,9 +5434,9 @@
       <c r="E109" s="32">
         <v>770</v>
       </c>
-      <c r="F109" s="106"/>
-      <c r="G109" s="94"/>
-      <c r="H109" s="91"/>
+      <c r="F109" s="150"/>
+      <c r="G109" s="105"/>
+      <c r="H109" s="146"/>
     </row>
     <row r="110" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="16"/>
@@ -5450,35 +5450,35 @@
       <c r="E110" s="32">
         <v>870</v>
       </c>
-      <c r="F110" s="106"/>
-      <c r="G110" s="94"/>
-      <c r="H110" s="91"/>
+      <c r="F110" s="150"/>
+      <c r="G110" s="105"/>
+      <c r="H110" s="146"/>
     </row>
     <row r="111" spans="1:8" ht="104.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="16"/>
       <c r="B111" s="17"/>
-      <c r="C111" s="107" t="s">
+      <c r="C111" s="154" t="s">
         <v>106</v>
       </c>
-      <c r="D111" s="109" t="s">
+      <c r="D111" s="156" t="s">
         <v>14</v>
       </c>
-      <c r="E111" s="111">
+      <c r="E111" s="158">
         <v>3500</v>
       </c>
-      <c r="F111" s="106"/>
-      <c r="G111" s="94"/>
-      <c r="H111" s="91"/>
+      <c r="F111" s="150"/>
+      <c r="G111" s="105"/>
+      <c r="H111" s="146"/>
     </row>
     <row r="112" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="16"/>
       <c r="B112" s="17"/>
-      <c r="C112" s="108"/>
-      <c r="D112" s="110"/>
-      <c r="E112" s="112"/>
-      <c r="F112" s="106"/>
-      <c r="G112" s="94"/>
-      <c r="H112" s="91"/>
+      <c r="C112" s="155"/>
+      <c r="D112" s="157"/>
+      <c r="E112" s="159"/>
+      <c r="F112" s="150"/>
+      <c r="G112" s="105"/>
+      <c r="H112" s="146"/>
     </row>
     <row r="113" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="16"/>
@@ -5492,9 +5492,9 @@
       <c r="E113" s="35">
         <v>2800</v>
       </c>
-      <c r="F113" s="106"/>
-      <c r="G113" s="94"/>
-      <c r="H113" s="91"/>
+      <c r="F113" s="150"/>
+      <c r="G113" s="105"/>
+      <c r="H113" s="146"/>
     </row>
     <row r="114" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="16"/>
@@ -5508,9 +5508,9 @@
       <c r="E114" s="35">
         <v>3300</v>
       </c>
-      <c r="F114" s="106"/>
-      <c r="G114" s="94"/>
-      <c r="H114" s="91"/>
+      <c r="F114" s="150"/>
+      <c r="G114" s="105"/>
+      <c r="H114" s="146"/>
     </row>
     <row r="115" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="16"/>
@@ -5524,9 +5524,9 @@
       <c r="E115" s="32">
         <v>980</v>
       </c>
-      <c r="F115" s="106"/>
-      <c r="G115" s="94"/>
-      <c r="H115" s="91"/>
+      <c r="F115" s="150"/>
+      <c r="G115" s="105"/>
+      <c r="H115" s="146"/>
     </row>
     <row r="116" spans="1:8" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="8"/>
@@ -5540,21 +5540,21 @@
       <c r="E116" s="38">
         <v>980</v>
       </c>
-      <c r="F116" s="106"/>
-      <c r="G116" s="94"/>
-      <c r="H116" s="91"/>
+      <c r="F116" s="150"/>
+      <c r="G116" s="105"/>
+      <c r="H116" s="146"/>
     </row>
     <row r="117" spans="1:8" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="8"/>
       <c r="B117" s="9"/>
-      <c r="C117" s="113" t="s">
+      <c r="C117" s="151" t="s">
         <v>113</v>
       </c>
-      <c r="D117" s="114"/>
-      <c r="E117" s="115"/>
-      <c r="F117" s="98"/>
-      <c r="G117" s="94"/>
-      <c r="H117" s="91"/>
+      <c r="D117" s="152"/>
+      <c r="E117" s="153"/>
+      <c r="F117" s="119"/>
+      <c r="G117" s="105"/>
+      <c r="H117" s="146"/>
     </row>
     <row r="118" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="8"/>
@@ -5568,9 +5568,9 @@
       <c r="E118" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="F118" s="106"/>
-      <c r="G118" s="94"/>
-      <c r="H118" s="91"/>
+      <c r="F118" s="150"/>
+      <c r="G118" s="105"/>
+      <c r="H118" s="146"/>
     </row>
     <row r="119" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="16"/>
@@ -5584,9 +5584,9 @@
       <c r="E119" s="30">
         <v>3000</v>
       </c>
-      <c r="F119" s="90"/>
-      <c r="G119" s="94"/>
-      <c r="H119" s="91"/>
+      <c r="F119" s="104"/>
+      <c r="G119" s="105"/>
+      <c r="H119" s="146"/>
     </row>
     <row r="120" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="16"/>
@@ -5600,9 +5600,9 @@
       <c r="E120" s="30">
         <v>3000</v>
       </c>
-      <c r="F120" s="90"/>
-      <c r="G120" s="94"/>
-      <c r="H120" s="91"/>
+      <c r="F120" s="104"/>
+      <c r="G120" s="105"/>
+      <c r="H120" s="146"/>
     </row>
     <row r="121" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="16"/>
@@ -5616,9 +5616,9 @@
       <c r="E121" s="30">
         <v>3000</v>
       </c>
-      <c r="F121" s="90"/>
-      <c r="G121" s="94"/>
-      <c r="H121" s="91"/>
+      <c r="F121" s="104"/>
+      <c r="G121" s="105"/>
+      <c r="H121" s="146"/>
     </row>
     <row r="122" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="16"/>
@@ -5632,9 +5632,9 @@
       <c r="E122" s="30">
         <v>3000</v>
       </c>
-      <c r="F122" s="90"/>
-      <c r="G122" s="94"/>
-      <c r="H122" s="91"/>
+      <c r="F122" s="104"/>
+      <c r="G122" s="105"/>
+      <c r="H122" s="146"/>
     </row>
     <row r="123" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="16"/>
@@ -5648,9 +5648,9 @@
       <c r="E123" s="30">
         <v>3000</v>
       </c>
-      <c r="F123" s="90"/>
-      <c r="G123" s="94"/>
-      <c r="H123" s="91"/>
+      <c r="F123" s="104"/>
+      <c r="G123" s="105"/>
+      <c r="H123" s="146"/>
     </row>
     <row r="124" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="16"/>
@@ -5664,21 +5664,21 @@
       <c r="E124" s="40">
         <v>3000</v>
       </c>
-      <c r="F124" s="90"/>
-      <c r="G124" s="94"/>
-      <c r="H124" s="91"/>
+      <c r="F124" s="104"/>
+      <c r="G124" s="105"/>
+      <c r="H124" s="146"/>
     </row>
     <row r="125" spans="1:8" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="8"/>
       <c r="B125" s="9"/>
-      <c r="C125" s="116" t="s">
+      <c r="C125" s="147" t="s">
         <v>122</v>
       </c>
-      <c r="D125" s="117"/>
-      <c r="E125" s="118"/>
-      <c r="F125" s="98"/>
-      <c r="G125" s="94"/>
-      <c r="H125" s="91"/>
+      <c r="D125" s="148"/>
+      <c r="E125" s="149"/>
+      <c r="F125" s="119"/>
+      <c r="G125" s="105"/>
+      <c r="H125" s="146"/>
     </row>
     <row r="126" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="8"/>
@@ -5692,8 +5692,8 @@
       <c r="E126" s="30">
         <v>1260</v>
       </c>
-      <c r="F126" s="90"/>
-      <c r="G126" s="91"/>
+      <c r="F126" s="104"/>
+      <c r="G126" s="146"/>
       <c r="H126" s="15"/>
     </row>
     <row r="127" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5708,9 +5708,9 @@
       <c r="E127" s="30">
         <v>1900</v>
       </c>
-      <c r="F127" s="90"/>
-      <c r="G127" s="94"/>
-      <c r="H127" s="91"/>
+      <c r="F127" s="104"/>
+      <c r="G127" s="105"/>
+      <c r="H127" s="146"/>
     </row>
     <row r="128" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="8"/>
@@ -5724,9 +5724,9 @@
       <c r="E128" s="30">
         <v>1560</v>
       </c>
-      <c r="F128" s="90"/>
-      <c r="G128" s="94"/>
-      <c r="H128" s="91"/>
+      <c r="F128" s="104"/>
+      <c r="G128" s="105"/>
+      <c r="H128" s="146"/>
     </row>
     <row r="129" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="16"/>
@@ -5740,8 +5740,8 @@
       <c r="E129" s="14">
         <v>2520</v>
       </c>
-      <c r="F129" s="90"/>
-      <c r="G129" s="91"/>
+      <c r="F129" s="104"/>
+      <c r="G129" s="146"/>
       <c r="H129" s="15"/>
     </row>
     <row r="130" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5756,9 +5756,9 @@
       <c r="E130" s="14">
         <v>16350</v>
       </c>
-      <c r="F130" s="90"/>
-      <c r="G130" s="94"/>
-      <c r="H130" s="91"/>
+      <c r="F130" s="104"/>
+      <c r="G130" s="105"/>
+      <c r="H130" s="146"/>
     </row>
     <row r="131" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="16"/>
@@ -5772,9 +5772,9 @@
       <c r="E131" s="14">
         <v>9750</v>
       </c>
-      <c r="F131" s="90"/>
-      <c r="G131" s="94"/>
-      <c r="H131" s="91"/>
+      <c r="F131" s="104"/>
+      <c r="G131" s="105"/>
+      <c r="H131" s="146"/>
     </row>
     <row r="132" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="16"/>
@@ -5788,9 +5788,9 @@
       <c r="E132" s="30">
         <v>6650</v>
       </c>
-      <c r="F132" s="90"/>
-      <c r="G132" s="94"/>
-      <c r="H132" s="91"/>
+      <c r="F132" s="104"/>
+      <c r="G132" s="105"/>
+      <c r="H132" s="146"/>
     </row>
     <row r="133" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="16"/>
@@ -5804,9 +5804,9 @@
       <c r="E133" s="41" t="s">
         <v>133</v>
       </c>
-      <c r="F133" s="90"/>
-      <c r="G133" s="94"/>
-      <c r="H133" s="91"/>
+      <c r="F133" s="104"/>
+      <c r="G133" s="105"/>
+      <c r="H133" s="146"/>
     </row>
     <row r="134" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="16"/>
@@ -5820,9 +5820,9 @@
       <c r="E134" s="41" t="s">
         <v>115</v>
       </c>
-      <c r="F134" s="90"/>
-      <c r="G134" s="94"/>
-      <c r="H134" s="91"/>
+      <c r="F134" s="104"/>
+      <c r="G134" s="105"/>
+      <c r="H134" s="146"/>
     </row>
     <row r="135" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="16"/>
@@ -5836,9 +5836,9 @@
       <c r="E135" s="30">
         <v>2190</v>
       </c>
-      <c r="F135" s="90"/>
-      <c r="G135" s="94"/>
-      <c r="H135" s="91"/>
+      <c r="F135" s="104"/>
+      <c r="G135" s="105"/>
+      <c r="H135" s="146"/>
     </row>
     <row r="136" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="16"/>
@@ -5852,9 +5852,9 @@
       <c r="E136" s="30">
         <v>1750</v>
       </c>
-      <c r="F136" s="90"/>
-      <c r="G136" s="94"/>
-      <c r="H136" s="119"/>
+      <c r="F136" s="104"/>
+      <c r="G136" s="105"/>
+      <c r="H136" s="106"/>
     </row>
     <row r="137" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="16"/>
@@ -5868,9 +5868,9 @@
       <c r="E137" s="30">
         <v>12130</v>
       </c>
-      <c r="F137" s="90"/>
-      <c r="G137" s="94"/>
-      <c r="H137" s="119"/>
+      <c r="F137" s="104"/>
+      <c r="G137" s="105"/>
+      <c r="H137" s="106"/>
     </row>
     <row r="138" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="16"/>
@@ -5884,9 +5884,9 @@
       <c r="E138" s="30">
         <v>1470</v>
       </c>
-      <c r="F138" s="90"/>
-      <c r="G138" s="94"/>
-      <c r="H138" s="119"/>
+      <c r="F138" s="104"/>
+      <c r="G138" s="105"/>
+      <c r="H138" s="106"/>
     </row>
     <row r="139" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="16"/>
@@ -5900,9 +5900,9 @@
       <c r="E139" s="30">
         <v>830</v>
       </c>
-      <c r="F139" s="90"/>
-      <c r="G139" s="94"/>
-      <c r="H139" s="119"/>
+      <c r="F139" s="104"/>
+      <c r="G139" s="105"/>
+      <c r="H139" s="106"/>
     </row>
     <row r="140" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="16"/>
@@ -5916,9 +5916,9 @@
       <c r="E140" s="30">
         <v>1030</v>
       </c>
-      <c r="F140" s="90"/>
-      <c r="G140" s="94"/>
-      <c r="H140" s="119"/>
+      <c r="F140" s="104"/>
+      <c r="G140" s="105"/>
+      <c r="H140" s="106"/>
     </row>
     <row r="141" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="16"/>
@@ -5932,9 +5932,9 @@
       <c r="E141" s="42" t="s">
         <v>115</v>
       </c>
-      <c r="F141" s="90"/>
-      <c r="G141" s="94"/>
-      <c r="H141" s="119"/>
+      <c r="F141" s="104"/>
+      <c r="G141" s="105"/>
+      <c r="H141" s="106"/>
     </row>
     <row r="142" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="16"/>
@@ -5948,8 +5948,8 @@
       <c r="E142" s="14">
         <v>2250</v>
       </c>
-      <c r="F142" s="120"/>
-      <c r="G142" s="121"/>
+      <c r="F142" s="138"/>
+      <c r="G142" s="139"/>
       <c r="H142" s="43"/>
     </row>
     <row r="143" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5964,9 +5964,9 @@
       <c r="E143" s="30">
         <v>1650</v>
       </c>
-      <c r="F143" s="90"/>
-      <c r="G143" s="94"/>
-      <c r="H143" s="119"/>
+      <c r="F143" s="104"/>
+      <c r="G143" s="105"/>
+      <c r="H143" s="106"/>
     </row>
     <row r="144" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="16"/>
@@ -5980,9 +5980,9 @@
       <c r="E144" s="41" t="s">
         <v>115</v>
       </c>
-      <c r="F144" s="90"/>
-      <c r="G144" s="94"/>
-      <c r="H144" s="119"/>
+      <c r="F144" s="104"/>
+      <c r="G144" s="105"/>
+      <c r="H144" s="106"/>
     </row>
     <row r="145" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="16"/>
@@ -5996,9 +5996,9 @@
       <c r="E145" s="30">
         <v>2800</v>
       </c>
-      <c r="F145" s="90"/>
-      <c r="G145" s="94"/>
-      <c r="H145" s="119"/>
+      <c r="F145" s="104"/>
+      <c r="G145" s="105"/>
+      <c r="H145" s="106"/>
     </row>
     <row r="146" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="16"/>
@@ -6012,9 +6012,9 @@
       <c r="E146" s="30">
         <v>7200</v>
       </c>
-      <c r="F146" s="90"/>
-      <c r="G146" s="94"/>
-      <c r="H146" s="119"/>
+      <c r="F146" s="104"/>
+      <c r="G146" s="105"/>
+      <c r="H146" s="106"/>
     </row>
     <row r="147" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" s="16"/>
@@ -6028,9 +6028,9 @@
       <c r="E147" s="30">
         <v>4300</v>
       </c>
-      <c r="F147" s="90"/>
-      <c r="G147" s="94"/>
-      <c r="H147" s="119"/>
+      <c r="F147" s="104"/>
+      <c r="G147" s="105"/>
+      <c r="H147" s="106"/>
     </row>
     <row r="148" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="16"/>
@@ -6044,9 +6044,9 @@
       <c r="E148" s="30">
         <v>7700</v>
       </c>
-      <c r="F148" s="90"/>
-      <c r="G148" s="94"/>
-      <c r="H148" s="119"/>
+      <c r="F148" s="104"/>
+      <c r="G148" s="105"/>
+      <c r="H148" s="106"/>
     </row>
     <row r="149" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="16"/>
@@ -6060,9 +6060,9 @@
       <c r="E149" s="14">
         <v>2760</v>
       </c>
-      <c r="F149" s="90"/>
-      <c r="G149" s="94"/>
-      <c r="H149" s="119"/>
+      <c r="F149" s="104"/>
+      <c r="G149" s="105"/>
+      <c r="H149" s="106"/>
     </row>
     <row r="150" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="16"/>
@@ -6076,9 +6076,9 @@
       <c r="E150" s="14">
         <v>1700</v>
       </c>
-      <c r="F150" s="90"/>
-      <c r="G150" s="94"/>
-      <c r="H150" s="119"/>
+      <c r="F150" s="104"/>
+      <c r="G150" s="105"/>
+      <c r="H150" s="106"/>
     </row>
     <row r="151" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="16"/>
@@ -6092,9 +6092,9 @@
       <c r="E151" s="14">
         <v>1080</v>
       </c>
-      <c r="F151" s="90"/>
-      <c r="G151" s="94"/>
-      <c r="H151" s="119"/>
+      <c r="F151" s="104"/>
+      <c r="G151" s="105"/>
+      <c r="H151" s="106"/>
     </row>
     <row r="152" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="16"/>
@@ -6108,21 +6108,21 @@
       <c r="E152" s="40">
         <v>2340</v>
       </c>
-      <c r="F152" s="90"/>
-      <c r="G152" s="94"/>
-      <c r="H152" s="119"/>
+      <c r="F152" s="104"/>
+      <c r="G152" s="105"/>
+      <c r="H152" s="106"/>
     </row>
     <row r="153" spans="1:8" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="8"/>
       <c r="B153" s="9"/>
-      <c r="C153" s="122" t="s">
+      <c r="C153" s="143" t="s">
         <v>157</v>
       </c>
-      <c r="D153" s="123"/>
-      <c r="E153" s="124"/>
-      <c r="F153" s="98"/>
-      <c r="G153" s="94"/>
-      <c r="H153" s="119"/>
+      <c r="D153" s="144"/>
+      <c r="E153" s="145"/>
+      <c r="F153" s="119"/>
+      <c r="G153" s="105"/>
+      <c r="H153" s="106"/>
     </row>
     <row r="154" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" s="16"/>
@@ -6136,9 +6136,9 @@
       <c r="E154" s="46">
         <v>5420</v>
       </c>
-      <c r="F154" s="90"/>
-      <c r="G154" s="94"/>
-      <c r="H154" s="119"/>
+      <c r="F154" s="104"/>
+      <c r="G154" s="105"/>
+      <c r="H154" s="106"/>
     </row>
     <row r="155" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="16"/>
@@ -6168,9 +6168,9 @@
       <c r="E156" s="46">
         <v>7600</v>
       </c>
-      <c r="F156" s="90"/>
-      <c r="G156" s="94"/>
-      <c r="H156" s="119"/>
+      <c r="F156" s="104"/>
+      <c r="G156" s="105"/>
+      <c r="H156" s="106"/>
     </row>
     <row r="157" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="16"/>
@@ -6184,9 +6184,9 @@
       <c r="E157" s="46">
         <v>8990</v>
       </c>
-      <c r="F157" s="90"/>
-      <c r="G157" s="94"/>
-      <c r="H157" s="119"/>
+      <c r="F157" s="104"/>
+      <c r="G157" s="105"/>
+      <c r="H157" s="106"/>
     </row>
     <row r="158" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="16"/>
@@ -6200,9 +6200,9 @@
       <c r="E158" s="46">
         <v>9500</v>
       </c>
-      <c r="F158" s="90"/>
-      <c r="G158" s="94"/>
-      <c r="H158" s="119"/>
+      <c r="F158" s="104"/>
+      <c r="G158" s="105"/>
+      <c r="H158" s="106"/>
     </row>
     <row r="159" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="16"/>
@@ -6216,9 +6216,9 @@
       <c r="E159" s="46">
         <v>9500</v>
       </c>
-      <c r="F159" s="90"/>
-      <c r="G159" s="94"/>
-      <c r="H159" s="119"/>
+      <c r="F159" s="104"/>
+      <c r="G159" s="105"/>
+      <c r="H159" s="106"/>
     </row>
     <row r="160" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="16"/>
@@ -6232,9 +6232,9 @@
       <c r="E160" s="46">
         <v>13200</v>
       </c>
-      <c r="F160" s="90"/>
-      <c r="G160" s="94"/>
-      <c r="H160" s="119"/>
+      <c r="F160" s="104"/>
+      <c r="G160" s="105"/>
+      <c r="H160" s="106"/>
     </row>
     <row r="161" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="16"/>
@@ -6344,9 +6344,9 @@
       <c r="E167" s="46">
         <v>5100</v>
       </c>
-      <c r="F167" s="90"/>
-      <c r="G167" s="94"/>
-      <c r="H167" s="119"/>
+      <c r="F167" s="104"/>
+      <c r="G167" s="105"/>
+      <c r="H167" s="106"/>
     </row>
     <row r="168" spans="1:8" ht="111" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="8"/>
@@ -6360,9 +6360,9 @@
       <c r="E168" s="46">
         <v>14680</v>
       </c>
-      <c r="F168" s="90"/>
-      <c r="G168" s="94"/>
-      <c r="H168" s="119"/>
+      <c r="F168" s="104"/>
+      <c r="G168" s="105"/>
+      <c r="H168" s="106"/>
     </row>
     <row r="169" spans="1:8" ht="111" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="8"/>
@@ -6376,9 +6376,9 @@
       <c r="E169" s="46">
         <v>13975</v>
       </c>
-      <c r="F169" s="90"/>
-      <c r="G169" s="94"/>
-      <c r="H169" s="119"/>
+      <c r="F169" s="104"/>
+      <c r="G169" s="105"/>
+      <c r="H169" s="106"/>
     </row>
     <row r="170" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="8"/>
@@ -6392,9 +6392,9 @@
       <c r="E170" s="46">
         <v>840</v>
       </c>
-      <c r="F170" s="90"/>
-      <c r="G170" s="94"/>
-      <c r="H170" s="119"/>
+      <c r="F170" s="104"/>
+      <c r="G170" s="105"/>
+      <c r="H170" s="106"/>
     </row>
     <row r="171" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="8"/>
@@ -6408,9 +6408,9 @@
       <c r="E171" s="14">
         <v>1780</v>
       </c>
-      <c r="F171" s="90"/>
-      <c r="G171" s="94"/>
-      <c r="H171" s="119"/>
+      <c r="F171" s="104"/>
+      <c r="G171" s="105"/>
+      <c r="H171" s="106"/>
     </row>
     <row r="172" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="8"/>
@@ -6424,9 +6424,9 @@
       <c r="E172" s="14">
         <v>880</v>
       </c>
-      <c r="F172" s="90"/>
-      <c r="G172" s="94"/>
-      <c r="H172" s="119"/>
+      <c r="F172" s="104"/>
+      <c r="G172" s="105"/>
+      <c r="H172" s="106"/>
     </row>
     <row r="173" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="8"/>
@@ -6440,21 +6440,21 @@
       <c r="E173" s="21">
         <v>3320</v>
       </c>
-      <c r="F173" s="120"/>
-      <c r="G173" s="121"/>
+      <c r="F173" s="138"/>
+      <c r="G173" s="139"/>
       <c r="H173" s="43"/>
     </row>
     <row r="174" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="8"/>
       <c r="B174" s="9"/>
-      <c r="C174" s="125" t="s">
+      <c r="C174" s="140" t="s">
         <v>182</v>
       </c>
-      <c r="D174" s="126"/>
-      <c r="E174" s="127"/>
-      <c r="F174" s="98"/>
-      <c r="G174" s="94"/>
-      <c r="H174" s="119"/>
+      <c r="D174" s="141"/>
+      <c r="E174" s="142"/>
+      <c r="F174" s="119"/>
+      <c r="G174" s="105"/>
+      <c r="H174" s="106"/>
     </row>
     <row r="175" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="16"/>
@@ -6468,9 +6468,9 @@
       <c r="E175" s="30">
         <v>8900</v>
       </c>
-      <c r="F175" s="90"/>
-      <c r="G175" s="94"/>
-      <c r="H175" s="119"/>
+      <c r="F175" s="104"/>
+      <c r="G175" s="105"/>
+      <c r="H175" s="106"/>
     </row>
     <row r="176" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A176" s="16"/>
@@ -6484,9 +6484,9 @@
       <c r="E176" s="30">
         <v>7350</v>
       </c>
-      <c r="F176" s="90"/>
-      <c r="G176" s="94"/>
-      <c r="H176" s="119"/>
+      <c r="F176" s="104"/>
+      <c r="G176" s="105"/>
+      <c r="H176" s="106"/>
     </row>
     <row r="177" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A177" s="16"/>
@@ -6500,9 +6500,9 @@
       <c r="E177" s="41" t="s">
         <v>115</v>
       </c>
-      <c r="F177" s="90"/>
-      <c r="G177" s="94"/>
-      <c r="H177" s="119"/>
+      <c r="F177" s="104"/>
+      <c r="G177" s="105"/>
+      <c r="H177" s="106"/>
     </row>
     <row r="178" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" s="16"/>
@@ -6516,9 +6516,9 @@
       <c r="E178" s="41" t="s">
         <v>115</v>
       </c>
-      <c r="F178" s="90"/>
-      <c r="G178" s="94"/>
-      <c r="H178" s="119"/>
+      <c r="F178" s="104"/>
+      <c r="G178" s="105"/>
+      <c r="H178" s="106"/>
     </row>
     <row r="179" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A179" s="16"/>
@@ -6532,9 +6532,9 @@
       <c r="E179" s="30">
         <v>8000</v>
       </c>
-      <c r="F179" s="90"/>
-      <c r="G179" s="94"/>
-      <c r="H179" s="119"/>
+      <c r="F179" s="104"/>
+      <c r="G179" s="105"/>
+      <c r="H179" s="106"/>
     </row>
     <row r="180" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A180" s="16"/>
@@ -6548,9 +6548,9 @@
       <c r="E180" s="30">
         <v>5850</v>
       </c>
-      <c r="F180" s="90"/>
-      <c r="G180" s="94"/>
-      <c r="H180" s="119"/>
+      <c r="F180" s="104"/>
+      <c r="G180" s="105"/>
+      <c r="H180" s="106"/>
     </row>
     <row r="181" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="16"/>
@@ -6564,47 +6564,47 @@
       <c r="E181" s="41" t="s">
         <v>115</v>
       </c>
-      <c r="F181" s="90"/>
-      <c r="G181" s="94"/>
-      <c r="H181" s="119"/>
+      <c r="F181" s="104"/>
+      <c r="G181" s="105"/>
+      <c r="H181" s="106"/>
     </row>
     <row r="182" spans="1:8" ht="119.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A182" s="16"/>
       <c r="B182" s="48"/>
-      <c r="C182" s="128" t="s">
+      <c r="C182" s="129" t="s">
         <v>193</v>
       </c>
-      <c r="D182" s="130" t="s">
+      <c r="D182" s="131" t="s">
         <v>90</v>
       </c>
-      <c r="E182" s="132" t="s">
+      <c r="E182" s="133" t="s">
         <v>133</v>
       </c>
-      <c r="F182" s="99"/>
-      <c r="G182" s="94"/>
-      <c r="H182" s="119"/>
+      <c r="F182" s="115"/>
+      <c r="G182" s="105"/>
+      <c r="H182" s="106"/>
     </row>
     <row r="183" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A183" s="16"/>
       <c r="B183" s="17"/>
-      <c r="C183" s="129"/>
-      <c r="D183" s="131"/>
-      <c r="E183" s="133"/>
-      <c r="F183" s="99"/>
-      <c r="G183" s="94"/>
-      <c r="H183" s="119"/>
+      <c r="C183" s="130"/>
+      <c r="D183" s="132"/>
+      <c r="E183" s="134"/>
+      <c r="F183" s="115"/>
+      <c r="G183" s="105"/>
+      <c r="H183" s="106"/>
     </row>
     <row r="184" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" s="8"/>
       <c r="B184" s="9"/>
-      <c r="C184" s="134" t="s">
+      <c r="C184" s="135" t="s">
         <v>194</v>
       </c>
-      <c r="D184" s="135"/>
-      <c r="E184" s="136"/>
-      <c r="F184" s="98"/>
-      <c r="G184" s="94"/>
-      <c r="H184" s="119"/>
+      <c r="D184" s="136"/>
+      <c r="E184" s="137"/>
+      <c r="F184" s="119"/>
+      <c r="G184" s="105"/>
+      <c r="H184" s="106"/>
     </row>
     <row r="185" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" s="16"/>
@@ -6618,9 +6618,9 @@
       <c r="E185" s="51">
         <v>700</v>
       </c>
-      <c r="F185" s="99"/>
-      <c r="G185" s="94"/>
-      <c r="H185" s="119"/>
+      <c r="F185" s="115"/>
+      <c r="G185" s="105"/>
+      <c r="H185" s="106"/>
     </row>
     <row r="186" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A186" s="16"/>
@@ -6634,9 +6634,9 @@
       <c r="E186" s="51">
         <v>630</v>
       </c>
-      <c r="F186" s="99"/>
-      <c r="G186" s="94"/>
-      <c r="H186" s="119"/>
+      <c r="F186" s="115"/>
+      <c r="G186" s="105"/>
+      <c r="H186" s="106"/>
     </row>
     <row r="187" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" s="16"/>
@@ -6650,9 +6650,9 @@
       <c r="E187" s="51">
         <v>500</v>
       </c>
-      <c r="F187" s="99"/>
-      <c r="G187" s="94"/>
-      <c r="H187" s="119"/>
+      <c r="F187" s="115"/>
+      <c r="G187" s="105"/>
+      <c r="H187" s="106"/>
     </row>
     <row r="188" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A188" s="16"/>
@@ -6666,9 +6666,9 @@
       <c r="E188" s="51">
         <v>600</v>
       </c>
-      <c r="F188" s="99"/>
-      <c r="G188" s="94"/>
-      <c r="H188" s="119"/>
+      <c r="F188" s="115"/>
+      <c r="G188" s="105"/>
+      <c r="H188" s="106"/>
     </row>
     <row r="189" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" s="16"/>
@@ -6682,9 +6682,9 @@
       <c r="E189" s="51">
         <v>500</v>
       </c>
-      <c r="F189" s="99"/>
-      <c r="G189" s="94"/>
-      <c r="H189" s="119"/>
+      <c r="F189" s="115"/>
+      <c r="G189" s="105"/>
+      <c r="H189" s="106"/>
     </row>
     <row r="190" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A190" s="16"/>
@@ -6698,9 +6698,9 @@
       <c r="E190" s="51">
         <v>825</v>
       </c>
-      <c r="F190" s="99"/>
-      <c r="G190" s="94"/>
-      <c r="H190" s="119"/>
+      <c r="F190" s="115"/>
+      <c r="G190" s="105"/>
+      <c r="H190" s="106"/>
     </row>
     <row r="191" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" s="16"/>
@@ -6714,9 +6714,9 @@
       <c r="E191" s="51">
         <v>890</v>
       </c>
-      <c r="F191" s="99"/>
-      <c r="G191" s="94"/>
-      <c r="H191" s="119"/>
+      <c r="F191" s="115"/>
+      <c r="G191" s="105"/>
+      <c r="H191" s="106"/>
     </row>
     <row r="192" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A192" s="16"/>
@@ -6730,9 +6730,9 @@
       <c r="E192" s="51">
         <v>970</v>
       </c>
-      <c r="F192" s="99"/>
-      <c r="G192" s="94"/>
-      <c r="H192" s="119"/>
+      <c r="F192" s="115"/>
+      <c r="G192" s="105"/>
+      <c r="H192" s="106"/>
     </row>
     <row r="193" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A193" s="16"/>
@@ -6746,9 +6746,9 @@
       <c r="E193" s="51">
         <v>950</v>
       </c>
-      <c r="F193" s="99"/>
-      <c r="G193" s="94"/>
-      <c r="H193" s="119"/>
+      <c r="F193" s="115"/>
+      <c r="G193" s="105"/>
+      <c r="H193" s="106"/>
     </row>
     <row r="194" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A194" s="16"/>
@@ -6762,9 +6762,9 @@
       <c r="E194" s="52" t="s">
         <v>115</v>
       </c>
-      <c r="F194" s="99"/>
-      <c r="G194" s="94"/>
-      <c r="H194" s="119"/>
+      <c r="F194" s="115"/>
+      <c r="G194" s="105"/>
+      <c r="H194" s="106"/>
     </row>
     <row r="195" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A195" s="16"/>
@@ -6778,9 +6778,9 @@
       <c r="E195" s="51">
         <v>1250</v>
       </c>
-      <c r="F195" s="99"/>
-      <c r="G195" s="94"/>
-      <c r="H195" s="119"/>
+      <c r="F195" s="115"/>
+      <c r="G195" s="105"/>
+      <c r="H195" s="106"/>
     </row>
     <row r="196" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A196" s="16"/>
@@ -6794,9 +6794,9 @@
       <c r="E196" s="51">
         <v>800</v>
       </c>
-      <c r="F196" s="99"/>
-      <c r="G196" s="94"/>
-      <c r="H196" s="119"/>
+      <c r="F196" s="115"/>
+      <c r="G196" s="105"/>
+      <c r="H196" s="106"/>
     </row>
     <row r="197" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A197" s="16"/>
@@ -6810,9 +6810,9 @@
       <c r="E197" s="51">
         <v>1020</v>
       </c>
-      <c r="F197" s="99"/>
-      <c r="G197" s="94"/>
-      <c r="H197" s="119"/>
+      <c r="F197" s="115"/>
+      <c r="G197" s="105"/>
+      <c r="H197" s="106"/>
     </row>
     <row r="198" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A198" s="16"/>
@@ -6826,9 +6826,9 @@
       <c r="E198" s="51">
         <v>500</v>
       </c>
-      <c r="F198" s="99"/>
-      <c r="G198" s="94"/>
-      <c r="H198" s="119"/>
+      <c r="F198" s="115"/>
+      <c r="G198" s="105"/>
+      <c r="H198" s="106"/>
     </row>
     <row r="199" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A199" s="16"/>
@@ -6842,9 +6842,9 @@
       <c r="E199" s="51">
         <v>620</v>
       </c>
-      <c r="F199" s="99"/>
-      <c r="G199" s="94"/>
-      <c r="H199" s="119"/>
+      <c r="F199" s="115"/>
+      <c r="G199" s="105"/>
+      <c r="H199" s="106"/>
     </row>
     <row r="200" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A200" s="16"/>
@@ -6858,9 +6858,9 @@
       <c r="E200" s="51">
         <v>910</v>
       </c>
-      <c r="F200" s="99"/>
-      <c r="G200" s="94"/>
-      <c r="H200" s="119"/>
+      <c r="F200" s="115"/>
+      <c r="G200" s="105"/>
+      <c r="H200" s="106"/>
     </row>
     <row r="201" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A201" s="16"/>
@@ -6874,9 +6874,9 @@
       <c r="E201" s="51">
         <v>935</v>
       </c>
-      <c r="F201" s="99"/>
-      <c r="G201" s="94"/>
-      <c r="H201" s="119"/>
+      <c r="F201" s="115"/>
+      <c r="G201" s="105"/>
+      <c r="H201" s="106"/>
     </row>
     <row r="202" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A202" s="16"/>
@@ -6890,32 +6890,32 @@
       <c r="E202" s="51">
         <v>1850</v>
       </c>
-      <c r="F202" s="99"/>
-      <c r="G202" s="94"/>
-      <c r="H202" s="119"/>
+      <c r="F202" s="115"/>
+      <c r="G202" s="105"/>
+      <c r="H202" s="106"/>
     </row>
     <row r="203" spans="1:8" ht="119.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A203" s="16"/>
       <c r="B203" s="17"/>
-      <c r="C203" s="137" t="s">
+      <c r="C203" s="123" t="s">
         <v>213</v>
       </c>
-      <c r="D203" s="139" t="s">
+      <c r="D203" s="125" t="s">
         <v>142</v>
       </c>
-      <c r="E203" s="141">
+      <c r="E203" s="127">
         <v>3350</v>
       </c>
-      <c r="F203" s="99"/>
-      <c r="G203" s="94"/>
-      <c r="H203" s="119"/>
+      <c r="F203" s="115"/>
+      <c r="G203" s="105"/>
+      <c r="H203" s="106"/>
     </row>
     <row r="204" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A204" s="16"/>
       <c r="B204" s="17"/>
-      <c r="C204" s="138"/>
-      <c r="D204" s="140"/>
-      <c r="E204" s="142"/>
+      <c r="C204" s="124"/>
+      <c r="D204" s="126"/>
+      <c r="E204" s="128"/>
       <c r="F204" s="43"/>
       <c r="G204" s="43"/>
       <c r="H204" s="43"/>
@@ -6932,9 +6932,9 @@
       <c r="E205" s="51">
         <v>1520</v>
       </c>
-      <c r="F205" s="99"/>
-      <c r="G205" s="94"/>
-      <c r="H205" s="119"/>
+      <c r="F205" s="115"/>
+      <c r="G205" s="105"/>
+      <c r="H205" s="106"/>
     </row>
     <row r="206" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A206" s="16"/>
@@ -6948,9 +6948,9 @@
       <c r="E206" s="51">
         <v>2050</v>
       </c>
-      <c r="F206" s="99"/>
-      <c r="G206" s="94"/>
-      <c r="H206" s="119"/>
+      <c r="F206" s="115"/>
+      <c r="G206" s="105"/>
+      <c r="H206" s="106"/>
     </row>
     <row r="207" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A207" s="16"/>
@@ -6964,9 +6964,9 @@
       <c r="E207" s="51">
         <v>1840</v>
       </c>
-      <c r="F207" s="99"/>
-      <c r="G207" s="94"/>
-      <c r="H207" s="119"/>
+      <c r="F207" s="115"/>
+      <c r="G207" s="105"/>
+      <c r="H207" s="106"/>
     </row>
     <row r="208" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A208" s="16"/>
@@ -6980,9 +6980,9 @@
       <c r="E208" s="51">
         <v>550</v>
       </c>
-      <c r="F208" s="99"/>
-      <c r="G208" s="94"/>
-      <c r="H208" s="119"/>
+      <c r="F208" s="115"/>
+      <c r="G208" s="105"/>
+      <c r="H208" s="106"/>
     </row>
     <row r="209" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A209" s="16"/>
@@ -6996,9 +6996,9 @@
       <c r="E209" s="51">
         <v>2900</v>
       </c>
-      <c r="F209" s="99"/>
-      <c r="G209" s="94"/>
-      <c r="H209" s="119"/>
+      <c r="F209" s="115"/>
+      <c r="G209" s="105"/>
+      <c r="H209" s="106"/>
     </row>
     <row r="210" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A210" s="16"/>
@@ -7012,9 +7012,9 @@
       <c r="E210" s="51">
         <v>1030</v>
       </c>
-      <c r="F210" s="99"/>
-      <c r="G210" s="94"/>
-      <c r="H210" s="119"/>
+      <c r="F210" s="115"/>
+      <c r="G210" s="105"/>
+      <c r="H210" s="106"/>
     </row>
     <row r="211" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A211" s="16"/>
@@ -7028,9 +7028,9 @@
       <c r="E211" s="51">
         <v>990</v>
       </c>
-      <c r="F211" s="99"/>
-      <c r="G211" s="94"/>
-      <c r="H211" s="119"/>
+      <c r="F211" s="115"/>
+      <c r="G211" s="105"/>
+      <c r="H211" s="106"/>
     </row>
     <row r="212" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A212" s="16"/>
@@ -7044,9 +7044,9 @@
       <c r="E212" s="51">
         <v>2400</v>
       </c>
-      <c r="F212" s="99"/>
-      <c r="G212" s="94"/>
-      <c r="H212" s="119"/>
+      <c r="F212" s="115"/>
+      <c r="G212" s="105"/>
+      <c r="H212" s="106"/>
     </row>
     <row r="213" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A213" s="16"/>
@@ -7060,9 +7060,9 @@
       <c r="E213" s="51">
         <v>950</v>
       </c>
-      <c r="F213" s="99"/>
-      <c r="G213" s="94"/>
-      <c r="H213" s="119"/>
+      <c r="F213" s="115"/>
+      <c r="G213" s="105"/>
+      <c r="H213" s="106"/>
     </row>
     <row r="214" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A214" s="16"/>
@@ -7076,21 +7076,21 @@
       <c r="E214" s="55">
         <v>2600</v>
       </c>
-      <c r="F214" s="90"/>
-      <c r="G214" s="94"/>
-      <c r="H214" s="119"/>
+      <c r="F214" s="104"/>
+      <c r="G214" s="105"/>
+      <c r="H214" s="106"/>
     </row>
     <row r="215" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A215" s="8"/>
       <c r="B215" s="9"/>
-      <c r="C215" s="143" t="s">
+      <c r="C215" s="120" t="s">
         <v>224</v>
       </c>
-      <c r="D215" s="144"/>
-      <c r="E215" s="145"/>
-      <c r="F215" s="98"/>
-      <c r="G215" s="94"/>
-      <c r="H215" s="119"/>
+      <c r="D215" s="121"/>
+      <c r="E215" s="122"/>
+      <c r="F215" s="119"/>
+      <c r="G215" s="105"/>
+      <c r="H215" s="106"/>
     </row>
     <row r="216" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A216" s="16"/>
@@ -7104,9 +7104,9 @@
       <c r="E216" s="14">
         <v>1490</v>
       </c>
-      <c r="F216" s="90"/>
-      <c r="G216" s="94"/>
-      <c r="H216" s="119"/>
+      <c r="F216" s="104"/>
+      <c r="G216" s="105"/>
+      <c r="H216" s="106"/>
     </row>
     <row r="217" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A217" s="16"/>
@@ -7120,9 +7120,9 @@
       <c r="E217" s="14">
         <v>1200</v>
       </c>
-      <c r="F217" s="90"/>
-      <c r="G217" s="94"/>
-      <c r="H217" s="119"/>
+      <c r="F217" s="104"/>
+      <c r="G217" s="105"/>
+      <c r="H217" s="106"/>
     </row>
     <row r="218" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A218" s="16"/>
@@ -7136,9 +7136,9 @@
       <c r="E218" s="14">
         <v>1720</v>
       </c>
-      <c r="F218" s="90"/>
-      <c r="G218" s="94"/>
-      <c r="H218" s="119"/>
+      <c r="F218" s="104"/>
+      <c r="G218" s="105"/>
+      <c r="H218" s="106"/>
     </row>
     <row r="219" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A219" s="16"/>
@@ -7152,9 +7152,9 @@
       <c r="E219" s="14">
         <v>830</v>
       </c>
-      <c r="F219" s="90"/>
-      <c r="G219" s="94"/>
-      <c r="H219" s="119"/>
+      <c r="F219" s="104"/>
+      <c r="G219" s="105"/>
+      <c r="H219" s="106"/>
     </row>
     <row r="220" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A220" s="16"/>
@@ -7168,9 +7168,9 @@
       <c r="E220" s="30">
         <v>2200</v>
       </c>
-      <c r="F220" s="90"/>
-      <c r="G220" s="94"/>
-      <c r="H220" s="119"/>
+      <c r="F220" s="104"/>
+      <c r="G220" s="105"/>
+      <c r="H220" s="106"/>
     </row>
     <row r="221" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A221" s="16"/>
@@ -7184,9 +7184,9 @@
       <c r="E221" s="30">
         <v>2000</v>
       </c>
-      <c r="F221" s="90"/>
-      <c r="G221" s="94"/>
-      <c r="H221" s="119"/>
+      <c r="F221" s="104"/>
+      <c r="G221" s="105"/>
+      <c r="H221" s="106"/>
     </row>
     <row r="222" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A222" s="16"/>
@@ -7200,9 +7200,9 @@
       <c r="E222" s="30">
         <v>1540</v>
       </c>
-      <c r="F222" s="90"/>
-      <c r="G222" s="94"/>
-      <c r="H222" s="119"/>
+      <c r="F222" s="104"/>
+      <c r="G222" s="105"/>
+      <c r="H222" s="106"/>
     </row>
     <row r="223" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A223" s="16"/>
@@ -7216,9 +7216,9 @@
       <c r="E223" s="30">
         <v>1140</v>
       </c>
-      <c r="F223" s="90"/>
-      <c r="G223" s="94"/>
-      <c r="H223" s="119"/>
+      <c r="F223" s="104"/>
+      <c r="G223" s="105"/>
+      <c r="H223" s="106"/>
     </row>
     <row r="224" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A224" s="16"/>
@@ -7232,9 +7232,9 @@
       <c r="E224" s="30">
         <v>1500</v>
       </c>
-      <c r="F224" s="90"/>
-      <c r="G224" s="94"/>
-      <c r="H224" s="119"/>
+      <c r="F224" s="104"/>
+      <c r="G224" s="105"/>
+      <c r="H224" s="106"/>
     </row>
     <row r="225" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A225" s="8"/>
@@ -7248,21 +7248,21 @@
       <c r="E225" s="26">
         <v>2170</v>
       </c>
-      <c r="F225" s="99"/>
-      <c r="G225" s="94"/>
-      <c r="H225" s="119"/>
+      <c r="F225" s="115"/>
+      <c r="G225" s="105"/>
+      <c r="H225" s="106"/>
     </row>
     <row r="226" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A226" s="8"/>
       <c r="B226" s="9"/>
-      <c r="C226" s="146" t="s">
+      <c r="C226" s="116" t="s">
         <v>235</v>
       </c>
-      <c r="D226" s="147"/>
-      <c r="E226" s="148"/>
-      <c r="F226" s="98"/>
-      <c r="G226" s="94"/>
-      <c r="H226" s="119"/>
+      <c r="D226" s="117"/>
+      <c r="E226" s="118"/>
+      <c r="F226" s="119"/>
+      <c r="G226" s="105"/>
+      <c r="H226" s="106"/>
     </row>
     <row r="227" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A227" s="16"/>
@@ -7276,9 +7276,9 @@
       <c r="E227" s="30">
         <v>1070</v>
       </c>
-      <c r="F227" s="90"/>
-      <c r="G227" s="94"/>
-      <c r="H227" s="119"/>
+      <c r="F227" s="104"/>
+      <c r="G227" s="105"/>
+      <c r="H227" s="106"/>
     </row>
     <row r="228" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A228" s="16"/>
@@ -7292,9 +7292,9 @@
       <c r="E228" s="30">
         <v>960</v>
       </c>
-      <c r="F228" s="90"/>
-      <c r="G228" s="94"/>
-      <c r="H228" s="119"/>
+      <c r="F228" s="104"/>
+      <c r="G228" s="105"/>
+      <c r="H228" s="106"/>
     </row>
     <row r="229" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A229" s="16"/>
@@ -7308,9 +7308,9 @@
       <c r="E229" s="30">
         <v>3800</v>
       </c>
-      <c r="F229" s="149"/>
-      <c r="G229" s="150"/>
-      <c r="H229" s="151"/>
+      <c r="F229" s="112"/>
+      <c r="G229" s="113"/>
+      <c r="H229" s="114"/>
     </row>
     <row r="230" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A230" s="16"/>
@@ -7324,9 +7324,9 @@
       <c r="E230" s="30">
         <v>1390</v>
       </c>
-      <c r="F230" s="90"/>
-      <c r="G230" s="94"/>
-      <c r="H230" s="119"/>
+      <c r="F230" s="104"/>
+      <c r="G230" s="105"/>
+      <c r="H230" s="106"/>
     </row>
     <row r="231" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A231" s="16"/>
@@ -7340,9 +7340,9 @@
       <c r="E231" s="30">
         <v>1320</v>
       </c>
-      <c r="F231" s="90"/>
-      <c r="G231" s="94"/>
-      <c r="H231" s="119"/>
+      <c r="F231" s="104"/>
+      <c r="G231" s="105"/>
+      <c r="H231" s="106"/>
     </row>
     <row r="232" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A232" s="16"/>
@@ -7356,9 +7356,9 @@
       <c r="E232" s="30">
         <v>850</v>
       </c>
-      <c r="F232" s="90"/>
-      <c r="G232" s="94"/>
-      <c r="H232" s="119"/>
+      <c r="F232" s="104"/>
+      <c r="G232" s="105"/>
+      <c r="H232" s="106"/>
     </row>
     <row r="233" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A233" s="16"/>
@@ -7372,9 +7372,9 @@
       <c r="E233" s="30">
         <v>990</v>
       </c>
-      <c r="F233" s="90"/>
-      <c r="G233" s="94"/>
-      <c r="H233" s="119"/>
+      <c r="F233" s="104"/>
+      <c r="G233" s="105"/>
+      <c r="H233" s="106"/>
     </row>
     <row r="234" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A234" s="16"/>
@@ -7388,9 +7388,9 @@
       <c r="E234" s="30">
         <v>920</v>
       </c>
-      <c r="F234" s="90"/>
-      <c r="G234" s="94"/>
-      <c r="H234" s="119"/>
+      <c r="F234" s="104"/>
+      <c r="G234" s="105"/>
+      <c r="H234" s="106"/>
     </row>
     <row r="235" spans="1:8" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A235" s="16"/>
@@ -7404,10 +7404,10 @@
       <c r="E235" s="30">
         <v>1600</v>
       </c>
-      <c r="F235" s="92" t="s">
+      <c r="F235" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="G235" s="93"/>
+      <c r="G235" s="103"/>
       <c r="H235" s="43"/>
     </row>
     <row r="236" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7422,9 +7422,9 @@
       <c r="E236" s="30">
         <v>1340</v>
       </c>
-      <c r="F236" s="90"/>
-      <c r="G236" s="94"/>
-      <c r="H236" s="119"/>
+      <c r="F236" s="104"/>
+      <c r="G236" s="105"/>
+      <c r="H236" s="106"/>
     </row>
     <row r="237" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A237" s="16"/>
@@ -7438,9 +7438,9 @@
       <c r="E237" s="14">
         <v>2150</v>
       </c>
-      <c r="F237" s="90"/>
-      <c r="G237" s="94"/>
-      <c r="H237" s="119"/>
+      <c r="F237" s="104"/>
+      <c r="G237" s="105"/>
+      <c r="H237" s="106"/>
     </row>
     <row r="238" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A238" s="16"/>
@@ -7454,420 +7454,420 @@
       <c r="E238" s="30">
         <v>750</v>
       </c>
-      <c r="F238" s="90"/>
-      <c r="G238" s="94"/>
-      <c r="H238" s="119"/>
+      <c r="F238" s="104"/>
+      <c r="G238" s="105"/>
+      <c r="H238" s="106"/>
     </row>
     <row r="239" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A239" s="152"/>
-      <c r="B239" s="153"/>
-      <c r="C239" s="153"/>
-      <c r="D239" s="153"/>
-      <c r="E239" s="153"/>
-      <c r="F239" s="153"/>
-      <c r="G239" s="153"/>
-      <c r="H239" s="154"/>
+      <c r="A239" s="107"/>
+      <c r="B239" s="108"/>
+      <c r="C239" s="108"/>
+      <c r="D239" s="108"/>
+      <c r="E239" s="108"/>
+      <c r="F239" s="108"/>
+      <c r="G239" s="108"/>
+      <c r="H239" s="69"/>
     </row>
     <row r="240" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A240" s="58"/>
-      <c r="B240" s="155" t="s">
+      <c r="B240" s="109" t="s">
         <v>247</v>
       </c>
-      <c r="C240" s="156"/>
-      <c r="D240" s="156"/>
-      <c r="E240" s="156"/>
-      <c r="F240" s="157"/>
+      <c r="C240" s="110"/>
+      <c r="D240" s="110"/>
+      <c r="E240" s="110"/>
+      <c r="F240" s="111"/>
       <c r="G240" s="43"/>
       <c r="H240" s="43"/>
     </row>
     <row r="241" spans="1:8" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A241" s="58"/>
-      <c r="B241" s="158" t="s">
+      <c r="B241" s="85" t="s">
         <v>248</v>
       </c>
-      <c r="C241" s="159"/>
-      <c r="D241" s="159"/>
-      <c r="E241" s="159"/>
-      <c r="F241" s="160"/>
+      <c r="C241" s="86"/>
+      <c r="D241" s="86"/>
+      <c r="E241" s="86"/>
+      <c r="F241" s="87"/>
       <c r="G241" s="43"/>
       <c r="H241" s="43"/>
     </row>
     <row r="242" spans="1:8" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A242" s="59"/>
-      <c r="B242" s="161" t="s">
+      <c r="B242" s="82" t="s">
         <v>249</v>
       </c>
-      <c r="C242" s="162"/>
-      <c r="D242" s="162"/>
-      <c r="E242" s="162"/>
-      <c r="F242" s="163"/>
+      <c r="C242" s="83"/>
+      <c r="D242" s="83"/>
+      <c r="E242" s="83"/>
+      <c r="F242" s="84"/>
       <c r="G242" s="43"/>
       <c r="H242" s="43"/>
     </row>
     <row r="243" spans="1:8" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A243" s="58"/>
-      <c r="B243" s="158" t="s">
+      <c r="B243" s="85" t="s">
         <v>250</v>
       </c>
-      <c r="C243" s="159"/>
-      <c r="D243" s="159"/>
-      <c r="E243" s="159"/>
-      <c r="F243" s="160"/>
+      <c r="C243" s="86"/>
+      <c r="D243" s="86"/>
+      <c r="E243" s="86"/>
+      <c r="F243" s="87"/>
       <c r="G243" s="43"/>
       <c r="H243" s="43"/>
     </row>
     <row r="244" spans="1:8" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A244" s="58"/>
-      <c r="B244" s="161" t="s">
+      <c r="B244" s="82" t="s">
         <v>251</v>
       </c>
-      <c r="C244" s="162"/>
-      <c r="D244" s="162"/>
-      <c r="E244" s="162"/>
-      <c r="F244" s="163"/>
+      <c r="C244" s="83"/>
+      <c r="D244" s="83"/>
+      <c r="E244" s="83"/>
+      <c r="F244" s="84"/>
       <c r="G244" s="43"/>
       <c r="H244" s="43"/>
     </row>
     <row r="245" spans="1:8" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A245" s="58"/>
-      <c r="B245" s="158" t="s">
+      <c r="B245" s="85" t="s">
         <v>252</v>
       </c>
-      <c r="C245" s="159"/>
-      <c r="D245" s="159"/>
-      <c r="E245" s="159"/>
-      <c r="F245" s="160"/>
+      <c r="C245" s="86"/>
+      <c r="D245" s="86"/>
+      <c r="E245" s="86"/>
+      <c r="F245" s="87"/>
       <c r="G245" s="43"/>
       <c r="H245" s="43"/>
     </row>
     <row r="246" spans="1:8" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A246" s="58"/>
-      <c r="B246" s="161" t="s">
+      <c r="B246" s="82" t="s">
         <v>253</v>
       </c>
-      <c r="C246" s="162"/>
-      <c r="D246" s="162"/>
-      <c r="E246" s="162"/>
-      <c r="F246" s="163"/>
+      <c r="C246" s="83"/>
+      <c r="D246" s="83"/>
+      <c r="E246" s="83"/>
+      <c r="F246" s="84"/>
       <c r="G246" s="43"/>
       <c r="H246" s="43"/>
     </row>
     <row r="247" spans="1:8" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A247" s="58"/>
-      <c r="B247" s="158" t="s">
+      <c r="B247" s="85" t="s">
         <v>254</v>
       </c>
-      <c r="C247" s="159"/>
-      <c r="D247" s="159"/>
-      <c r="E247" s="159"/>
-      <c r="F247" s="160"/>
+      <c r="C247" s="86"/>
+      <c r="D247" s="86"/>
+      <c r="E247" s="86"/>
+      <c r="F247" s="87"/>
       <c r="G247" s="43"/>
       <c r="H247" s="43"/>
     </row>
     <row r="248" spans="1:8" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A248" s="58"/>
-      <c r="B248" s="161" t="s">
+      <c r="B248" s="82" t="s">
         <v>255</v>
       </c>
-      <c r="C248" s="162"/>
-      <c r="D248" s="162"/>
-      <c r="E248" s="162"/>
-      <c r="F248" s="163"/>
+      <c r="C248" s="83"/>
+      <c r="D248" s="83"/>
+      <c r="E248" s="83"/>
+      <c r="F248" s="84"/>
       <c r="G248" s="43"/>
       <c r="H248" s="43"/>
     </row>
     <row r="249" spans="1:8" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A249" s="58"/>
-      <c r="B249" s="158" t="s">
+      <c r="B249" s="85" t="s">
         <v>256</v>
       </c>
-      <c r="C249" s="159"/>
-      <c r="D249" s="159"/>
-      <c r="E249" s="159"/>
-      <c r="F249" s="160"/>
+      <c r="C249" s="86"/>
+      <c r="D249" s="86"/>
+      <c r="E249" s="86"/>
+      <c r="F249" s="87"/>
       <c r="G249" s="43"/>
       <c r="H249" s="43"/>
     </row>
     <row r="250" spans="1:8" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A250" s="58"/>
-      <c r="B250" s="161" t="s">
+      <c r="B250" s="82" t="s">
         <v>257</v>
       </c>
-      <c r="C250" s="162"/>
-      <c r="D250" s="162"/>
-      <c r="E250" s="162"/>
-      <c r="F250" s="163"/>
+      <c r="C250" s="83"/>
+      <c r="D250" s="83"/>
+      <c r="E250" s="83"/>
+      <c r="F250" s="84"/>
       <c r="G250" s="43"/>
       <c r="H250" s="43"/>
     </row>
     <row r="251" spans="1:8" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A251" s="58"/>
-      <c r="B251" s="158" t="s">
+      <c r="B251" s="85" t="s">
         <v>258</v>
       </c>
-      <c r="C251" s="159"/>
-      <c r="D251" s="159"/>
-      <c r="E251" s="159"/>
-      <c r="F251" s="160"/>
+      <c r="C251" s="86"/>
+      <c r="D251" s="86"/>
+      <c r="E251" s="86"/>
+      <c r="F251" s="87"/>
       <c r="G251" s="43"/>
       <c r="H251" s="43"/>
     </row>
     <row r="252" spans="1:8" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A252" s="60"/>
-      <c r="B252" s="164" t="s">
+      <c r="B252" s="99" t="s">
         <v>259</v>
       </c>
-      <c r="C252" s="165"/>
-      <c r="D252" s="165"/>
-      <c r="E252" s="165"/>
-      <c r="F252" s="166"/>
+      <c r="C252" s="100"/>
+      <c r="D252" s="100"/>
+      <c r="E252" s="100"/>
+      <c r="F252" s="101"/>
       <c r="G252" s="43"/>
       <c r="H252" s="43"/>
     </row>
     <row r="253" spans="1:8" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A253" s="60"/>
-      <c r="B253" s="167" t="s">
+      <c r="B253" s="96" t="s">
         <v>260</v>
       </c>
-      <c r="C253" s="168"/>
-      <c r="D253" s="168"/>
-      <c r="E253" s="168"/>
-      <c r="F253" s="169"/>
+      <c r="C253" s="97"/>
+      <c r="D253" s="97"/>
+      <c r="E253" s="97"/>
+      <c r="F253" s="98"/>
       <c r="G253" s="43"/>
       <c r="H253" s="43"/>
     </row>
     <row r="254" spans="1:8" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A254" s="58"/>
-      <c r="B254" s="161" t="s">
+      <c r="B254" s="82" t="s">
         <v>261</v>
       </c>
-      <c r="C254" s="162"/>
-      <c r="D254" s="162"/>
-      <c r="E254" s="162"/>
-      <c r="F254" s="163"/>
+      <c r="C254" s="83"/>
+      <c r="D254" s="83"/>
+      <c r="E254" s="83"/>
+      <c r="F254" s="84"/>
       <c r="G254" s="43"/>
       <c r="H254" s="43"/>
     </row>
     <row r="255" spans="1:8" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A255" s="59"/>
-      <c r="B255" s="158" t="s">
+      <c r="B255" s="85" t="s">
         <v>262</v>
       </c>
-      <c r="C255" s="159"/>
-      <c r="D255" s="159"/>
-      <c r="E255" s="159"/>
-      <c r="F255" s="160"/>
+      <c r="C255" s="86"/>
+      <c r="D255" s="86"/>
+      <c r="E255" s="86"/>
+      <c r="F255" s="87"/>
       <c r="G255" s="43"/>
       <c r="H255" s="43"/>
     </row>
     <row r="256" spans="1:8" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A256" s="61"/>
-      <c r="B256" s="161" t="s">
+      <c r="B256" s="82" t="s">
         <v>263</v>
       </c>
-      <c r="C256" s="162"/>
-      <c r="D256" s="162"/>
-      <c r="E256" s="162"/>
-      <c r="F256" s="163"/>
+      <c r="C256" s="83"/>
+      <c r="D256" s="83"/>
+      <c r="E256" s="83"/>
+      <c r="F256" s="84"/>
       <c r="G256" s="43"/>
       <c r="H256" s="43"/>
     </row>
     <row r="257" spans="1:8" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A257" s="58"/>
-      <c r="B257" s="158" t="s">
+      <c r="B257" s="85" t="s">
         <v>264</v>
       </c>
-      <c r="C257" s="159"/>
-      <c r="D257" s="159"/>
-      <c r="E257" s="159"/>
-      <c r="F257" s="160"/>
+      <c r="C257" s="86"/>
+      <c r="D257" s="86"/>
+      <c r="E257" s="86"/>
+      <c r="F257" s="87"/>
       <c r="G257" s="43"/>
       <c r="H257" s="43"/>
     </row>
     <row r="258" spans="1:8" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A258" s="61"/>
-      <c r="B258" s="158" t="s">
+      <c r="B258" s="85" t="s">
         <v>265</v>
       </c>
-      <c r="C258" s="159"/>
-      <c r="D258" s="159"/>
-      <c r="E258" s="159"/>
-      <c r="F258" s="160"/>
+      <c r="C258" s="86"/>
+      <c r="D258" s="86"/>
+      <c r="E258" s="86"/>
+      <c r="F258" s="87"/>
       <c r="G258" s="43"/>
       <c r="H258" s="43"/>
     </row>
     <row r="259" spans="1:8" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A259" s="59"/>
-      <c r="B259" s="161" t="s">
+      <c r="B259" s="82" t="s">
         <v>266</v>
       </c>
-      <c r="C259" s="162"/>
-      <c r="D259" s="162"/>
-      <c r="E259" s="162"/>
-      <c r="F259" s="163"/>
+      <c r="C259" s="83"/>
+      <c r="D259" s="83"/>
+      <c r="E259" s="83"/>
+      <c r="F259" s="84"/>
       <c r="G259" s="43"/>
       <c r="H259" s="43"/>
     </row>
     <row r="260" spans="1:8" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A260" s="58"/>
-      <c r="B260" s="158" t="s">
+      <c r="B260" s="85" t="s">
         <v>267</v>
       </c>
-      <c r="C260" s="159"/>
-      <c r="D260" s="159"/>
-      <c r="E260" s="159"/>
-      <c r="F260" s="160"/>
+      <c r="C260" s="86"/>
+      <c r="D260" s="86"/>
+      <c r="E260" s="86"/>
+      <c r="F260" s="87"/>
       <c r="G260" s="7"/>
       <c r="H260" s="7"/>
     </row>
     <row r="261" spans="1:8" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A261" s="58"/>
-      <c r="B261" s="161" t="s">
+      <c r="B261" s="82" t="s">
         <v>268</v>
       </c>
-      <c r="C261" s="162"/>
-      <c r="D261" s="162"/>
-      <c r="E261" s="162"/>
-      <c r="F261" s="163"/>
+      <c r="C261" s="83"/>
+      <c r="D261" s="83"/>
+      <c r="E261" s="83"/>
+      <c r="F261" s="84"/>
       <c r="G261" s="7"/>
       <c r="H261" s="7"/>
     </row>
     <row r="262" spans="1:8" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A262" s="58"/>
-      <c r="B262" s="158" t="s">
+      <c r="B262" s="85" t="s">
         <v>269</v>
       </c>
-      <c r="C262" s="159"/>
-      <c r="D262" s="159"/>
-      <c r="E262" s="159"/>
-      <c r="F262" s="160"/>
+      <c r="C262" s="86"/>
+      <c r="D262" s="86"/>
+      <c r="E262" s="86"/>
+      <c r="F262" s="87"/>
       <c r="G262" s="7"/>
       <c r="H262" s="7"/>
     </row>
     <row r="263" spans="1:8" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A263" s="58"/>
-      <c r="B263" s="161" t="s">
+      <c r="B263" s="82" t="s">
         <v>270</v>
       </c>
-      <c r="C263" s="162"/>
-      <c r="D263" s="162"/>
-      <c r="E263" s="162"/>
-      <c r="F263" s="163"/>
+      <c r="C263" s="83"/>
+      <c r="D263" s="83"/>
+      <c r="E263" s="83"/>
+      <c r="F263" s="84"/>
       <c r="G263" s="7"/>
       <c r="H263" s="7"/>
     </row>
     <row r="264" spans="1:8" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A264" s="58"/>
-      <c r="B264" s="158" t="s">
+      <c r="B264" s="85" t="s">
         <v>271</v>
       </c>
-      <c r="C264" s="159"/>
-      <c r="D264" s="159"/>
-      <c r="E264" s="159"/>
-      <c r="F264" s="160"/>
+      <c r="C264" s="86"/>
+      <c r="D264" s="86"/>
+      <c r="E264" s="86"/>
+      <c r="F264" s="87"/>
       <c r="G264" s="7"/>
       <c r="H264" s="7"/>
     </row>
     <row r="265" spans="1:8" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A265" s="58"/>
-      <c r="B265" s="161" t="s">
+      <c r="B265" s="82" t="s">
         <v>272</v>
       </c>
-      <c r="C265" s="162"/>
-      <c r="D265" s="162"/>
-      <c r="E265" s="162"/>
-      <c r="F265" s="163"/>
+      <c r="C265" s="83"/>
+      <c r="D265" s="83"/>
+      <c r="E265" s="83"/>
+      <c r="F265" s="84"/>
       <c r="G265" s="7"/>
       <c r="H265" s="7"/>
     </row>
     <row r="266" spans="1:8" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A266" s="58"/>
-      <c r="B266" s="158" t="s">
+      <c r="B266" s="85" t="s">
         <v>273</v>
       </c>
-      <c r="C266" s="159"/>
-      <c r="D266" s="159"/>
-      <c r="E266" s="159"/>
-      <c r="F266" s="160"/>
+      <c r="C266" s="86"/>
+      <c r="D266" s="86"/>
+      <c r="E266" s="86"/>
+      <c r="F266" s="87"/>
       <c r="G266" s="7"/>
       <c r="H266" s="7"/>
     </row>
     <row r="267" spans="1:8" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A267" s="58"/>
-      <c r="B267" s="161" t="s">
+      <c r="B267" s="82" t="s">
         <v>274</v>
       </c>
-      <c r="C267" s="162"/>
-      <c r="D267" s="162"/>
-      <c r="E267" s="162"/>
-      <c r="F267" s="163"/>
+      <c r="C267" s="83"/>
+      <c r="D267" s="83"/>
+      <c r="E267" s="83"/>
+      <c r="F267" s="84"/>
       <c r="G267" s="7"/>
       <c r="H267" s="7"/>
     </row>
     <row r="268" spans="1:8" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A268" s="58"/>
-      <c r="B268" s="158" t="s">
+      <c r="B268" s="85" t="s">
         <v>275</v>
       </c>
-      <c r="C268" s="159"/>
-      <c r="D268" s="159"/>
-      <c r="E268" s="159"/>
-      <c r="F268" s="160"/>
+      <c r="C268" s="86"/>
+      <c r="D268" s="86"/>
+      <c r="E268" s="86"/>
+      <c r="F268" s="87"/>
       <c r="G268" s="7"/>
       <c r="H268" s="7"/>
     </row>
     <row r="269" spans="1:8" ht="29.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A269" s="170"/>
-      <c r="B269" s="172" t="s">
+      <c r="A269" s="88"/>
+      <c r="B269" s="90" t="s">
         <v>276</v>
       </c>
-      <c r="C269" s="173"/>
-      <c r="D269" s="173"/>
-      <c r="E269" s="173"/>
-      <c r="F269" s="174"/>
-      <c r="G269" s="178"/>
-      <c r="H269" s="179"/>
+      <c r="C269" s="91"/>
+      <c r="D269" s="91"/>
+      <c r="E269" s="91"/>
+      <c r="F269" s="92"/>
+      <c r="G269" s="66"/>
+      <c r="H269" s="67"/>
     </row>
     <row r="270" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A270" s="171"/>
-      <c r="B270" s="175"/>
-      <c r="C270" s="176"/>
-      <c r="D270" s="176"/>
-      <c r="E270" s="176"/>
-      <c r="F270" s="177"/>
-      <c r="G270" s="180"/>
-      <c r="H270" s="154"/>
+      <c r="A270" s="89"/>
+      <c r="B270" s="93"/>
+      <c r="C270" s="94"/>
+      <c r="D270" s="94"/>
+      <c r="E270" s="94"/>
+      <c r="F270" s="95"/>
+      <c r="G270" s="68"/>
+      <c r="H270" s="69"/>
     </row>
     <row r="271" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A271" s="62"/>
-      <c r="B271" s="181" t="s">
+      <c r="B271" s="70" t="s">
         <v>277</v>
       </c>
-      <c r="C271" s="182"/>
-      <c r="D271" s="182"/>
-      <c r="E271" s="182"/>
-      <c r="F271" s="183"/>
+      <c r="C271" s="71"/>
+      <c r="D271" s="71"/>
+      <c r="E271" s="71"/>
+      <c r="F271" s="72"/>
       <c r="G271" s="63"/>
       <c r="H271" s="63"/>
     </row>
     <row r="272" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A272" s="62"/>
-      <c r="B272" s="184"/>
-      <c r="C272" s="185"/>
-      <c r="D272" s="185"/>
-      <c r="E272" s="185"/>
-      <c r="F272" s="186"/>
+      <c r="B272" s="73"/>
+      <c r="C272" s="74"/>
+      <c r="D272" s="74"/>
+      <c r="E272" s="74"/>
+      <c r="F272" s="75"/>
       <c r="G272" s="64"/>
       <c r="H272" s="64"/>
     </row>
     <row r="273" spans="1:8" ht="47.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A273" s="64"/>
       <c r="B273" s="65"/>
-      <c r="C273" s="187" t="s">
+      <c r="C273" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="D273" s="188"/>
-      <c r="E273" s="189"/>
+      <c r="D273" s="77"/>
+      <c r="E273" s="78"/>
       <c r="F273" s="64"/>
       <c r="G273" s="64"/>
       <c r="H273" s="64"/>
@@ -7875,111 +7875,198 @@
     <row r="274" spans="1:8" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A274" s="64"/>
       <c r="B274" s="65"/>
-      <c r="C274" s="190" t="s">
+      <c r="C274" s="79" t="s">
         <v>278</v>
       </c>
-      <c r="D274" s="191"/>
-      <c r="E274" s="192"/>
+      <c r="D274" s="80"/>
+      <c r="E274" s="81"/>
       <c r="F274" s="64"/>
       <c r="G274" s="64"/>
       <c r="H274" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="288">
-    <mergeCell ref="G269:H270"/>
-    <mergeCell ref="B271:F272"/>
-    <mergeCell ref="C273:E273"/>
-    <mergeCell ref="C274:E274"/>
-    <mergeCell ref="B265:F265"/>
-    <mergeCell ref="B266:F266"/>
-    <mergeCell ref="B267:F267"/>
-    <mergeCell ref="B268:F268"/>
-    <mergeCell ref="A269:A270"/>
-    <mergeCell ref="B269:F270"/>
-    <mergeCell ref="B259:F259"/>
-    <mergeCell ref="B260:F260"/>
-    <mergeCell ref="B261:F261"/>
-    <mergeCell ref="B262:F262"/>
-    <mergeCell ref="B263:F263"/>
-    <mergeCell ref="B264:F264"/>
-    <mergeCell ref="B253:F253"/>
-    <mergeCell ref="B254:F254"/>
-    <mergeCell ref="B255:F255"/>
-    <mergeCell ref="B256:F256"/>
-    <mergeCell ref="B257:F257"/>
-    <mergeCell ref="B258:F258"/>
-    <mergeCell ref="B247:F247"/>
-    <mergeCell ref="B248:F248"/>
-    <mergeCell ref="B249:F249"/>
-    <mergeCell ref="B250:F250"/>
-    <mergeCell ref="B251:F251"/>
-    <mergeCell ref="B252:F252"/>
-    <mergeCell ref="B241:F241"/>
-    <mergeCell ref="B242:F242"/>
-    <mergeCell ref="B243:F243"/>
-    <mergeCell ref="B244:F244"/>
-    <mergeCell ref="B245:F245"/>
-    <mergeCell ref="B246:F246"/>
-    <mergeCell ref="F235:G235"/>
-    <mergeCell ref="F236:H236"/>
-    <mergeCell ref="F237:H237"/>
-    <mergeCell ref="F238:H238"/>
-    <mergeCell ref="A239:H239"/>
-    <mergeCell ref="B240:F240"/>
-    <mergeCell ref="F229:H229"/>
-    <mergeCell ref="F230:H230"/>
-    <mergeCell ref="F231:H231"/>
-    <mergeCell ref="F232:H232"/>
-    <mergeCell ref="F233:H233"/>
-    <mergeCell ref="F234:H234"/>
-    <mergeCell ref="F224:H224"/>
-    <mergeCell ref="F225:H225"/>
-    <mergeCell ref="C226:E226"/>
-    <mergeCell ref="F226:H226"/>
-    <mergeCell ref="F227:H227"/>
-    <mergeCell ref="F228:H228"/>
-    <mergeCell ref="F218:H218"/>
-    <mergeCell ref="F219:H219"/>
-    <mergeCell ref="F220:H220"/>
-    <mergeCell ref="F221:H221"/>
-    <mergeCell ref="F222:H222"/>
-    <mergeCell ref="F223:H223"/>
-    <mergeCell ref="F213:H213"/>
-    <mergeCell ref="F214:H214"/>
-    <mergeCell ref="C215:E215"/>
-    <mergeCell ref="F215:H215"/>
-    <mergeCell ref="F216:H216"/>
-    <mergeCell ref="F217:H217"/>
-    <mergeCell ref="F207:H207"/>
-    <mergeCell ref="F208:H208"/>
-    <mergeCell ref="F209:H209"/>
-    <mergeCell ref="F210:H210"/>
-    <mergeCell ref="F211:H211"/>
-    <mergeCell ref="F212:H212"/>
-    <mergeCell ref="C203:C204"/>
-    <mergeCell ref="D203:D204"/>
-    <mergeCell ref="E203:E204"/>
-    <mergeCell ref="F203:H203"/>
-    <mergeCell ref="F205:H205"/>
-    <mergeCell ref="F206:H206"/>
-    <mergeCell ref="F197:H197"/>
-    <mergeCell ref="F198:H198"/>
-    <mergeCell ref="F199:H199"/>
-    <mergeCell ref="F200:H200"/>
-    <mergeCell ref="F201:H201"/>
-    <mergeCell ref="F202:H202"/>
-    <mergeCell ref="F191:H191"/>
-    <mergeCell ref="F192:H192"/>
-    <mergeCell ref="F193:H193"/>
-    <mergeCell ref="F194:H194"/>
-    <mergeCell ref="F195:H195"/>
-    <mergeCell ref="F196:H196"/>
-    <mergeCell ref="F185:H185"/>
-    <mergeCell ref="F186:H186"/>
-    <mergeCell ref="F187:H187"/>
-    <mergeCell ref="F188:H188"/>
-    <mergeCell ref="F189:H189"/>
-    <mergeCell ref="F190:H190"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="F45:H45"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="F46:H46"/>
+    <mergeCell ref="F47:H47"/>
+    <mergeCell ref="F48:H48"/>
+    <mergeCell ref="F49:H49"/>
+    <mergeCell ref="F39:H39"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="F56:H56"/>
+    <mergeCell ref="F57:H57"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="F59:H59"/>
+    <mergeCell ref="F60:H60"/>
+    <mergeCell ref="F61:H61"/>
+    <mergeCell ref="F50:H50"/>
+    <mergeCell ref="F51:H51"/>
+    <mergeCell ref="F52:H52"/>
+    <mergeCell ref="F53:H53"/>
+    <mergeCell ref="F54:H54"/>
+    <mergeCell ref="F55:H55"/>
+    <mergeCell ref="F68:H68"/>
+    <mergeCell ref="F69:H69"/>
+    <mergeCell ref="F70:H70"/>
+    <mergeCell ref="F71:G71"/>
+    <mergeCell ref="F72:H72"/>
+    <mergeCell ref="F73:H73"/>
+    <mergeCell ref="F62:H62"/>
+    <mergeCell ref="F63:H63"/>
+    <mergeCell ref="F64:H64"/>
+    <mergeCell ref="F65:H65"/>
+    <mergeCell ref="F66:H66"/>
+    <mergeCell ref="F67:H67"/>
+    <mergeCell ref="F80:H80"/>
+    <mergeCell ref="F81:H81"/>
+    <mergeCell ref="F82:H82"/>
+    <mergeCell ref="F83:H83"/>
+    <mergeCell ref="C84:E84"/>
+    <mergeCell ref="F84:H84"/>
+    <mergeCell ref="F74:H74"/>
+    <mergeCell ref="F75:H75"/>
+    <mergeCell ref="F76:H76"/>
+    <mergeCell ref="F77:H77"/>
+    <mergeCell ref="F78:H78"/>
+    <mergeCell ref="F79:H79"/>
+    <mergeCell ref="F91:G91"/>
+    <mergeCell ref="F92:H92"/>
+    <mergeCell ref="F93:H93"/>
+    <mergeCell ref="F94:H94"/>
+    <mergeCell ref="F95:G95"/>
+    <mergeCell ref="F96:G96"/>
+    <mergeCell ref="F85:G85"/>
+    <mergeCell ref="F86:H86"/>
+    <mergeCell ref="F87:H87"/>
+    <mergeCell ref="F88:H88"/>
+    <mergeCell ref="F89:H89"/>
+    <mergeCell ref="F90:G90"/>
+    <mergeCell ref="F103:H103"/>
+    <mergeCell ref="F104:H104"/>
+    <mergeCell ref="F105:H105"/>
+    <mergeCell ref="F106:H106"/>
+    <mergeCell ref="F107:H107"/>
+    <mergeCell ref="F108:H108"/>
+    <mergeCell ref="F97:H97"/>
+    <mergeCell ref="F98:G98"/>
+    <mergeCell ref="F99:H99"/>
+    <mergeCell ref="F100:H100"/>
+    <mergeCell ref="F101:H101"/>
+    <mergeCell ref="F102:H102"/>
+    <mergeCell ref="C117:E117"/>
+    <mergeCell ref="F117:H117"/>
+    <mergeCell ref="F109:H109"/>
+    <mergeCell ref="F110:H110"/>
+    <mergeCell ref="C111:C112"/>
+    <mergeCell ref="D111:D112"/>
+    <mergeCell ref="E111:E112"/>
+    <mergeCell ref="F111:H111"/>
+    <mergeCell ref="F112:H112"/>
+    <mergeCell ref="F118:H118"/>
+    <mergeCell ref="F119:H119"/>
+    <mergeCell ref="F120:H120"/>
+    <mergeCell ref="F121:H121"/>
+    <mergeCell ref="F122:H122"/>
+    <mergeCell ref="F123:H123"/>
+    <mergeCell ref="F113:H113"/>
+    <mergeCell ref="F114:H114"/>
+    <mergeCell ref="F115:H115"/>
+    <mergeCell ref="F116:H116"/>
+    <mergeCell ref="F129:G129"/>
+    <mergeCell ref="F130:H130"/>
+    <mergeCell ref="F131:H131"/>
+    <mergeCell ref="F132:H132"/>
+    <mergeCell ref="F133:H133"/>
+    <mergeCell ref="F134:H134"/>
+    <mergeCell ref="F124:H124"/>
+    <mergeCell ref="C125:E125"/>
+    <mergeCell ref="F125:H125"/>
+    <mergeCell ref="F126:G126"/>
+    <mergeCell ref="F127:H127"/>
+    <mergeCell ref="F128:H128"/>
+    <mergeCell ref="F141:H141"/>
+    <mergeCell ref="F142:G142"/>
+    <mergeCell ref="F143:H143"/>
+    <mergeCell ref="F144:H144"/>
+    <mergeCell ref="F145:H145"/>
+    <mergeCell ref="F146:H146"/>
+    <mergeCell ref="F135:H135"/>
+    <mergeCell ref="F136:H136"/>
+    <mergeCell ref="F137:H137"/>
+    <mergeCell ref="F138:H138"/>
+    <mergeCell ref="F139:H139"/>
+    <mergeCell ref="F140:H140"/>
+    <mergeCell ref="C153:E153"/>
+    <mergeCell ref="F153:H153"/>
+    <mergeCell ref="F154:H154"/>
+    <mergeCell ref="F156:H156"/>
+    <mergeCell ref="F157:H157"/>
+    <mergeCell ref="F158:H158"/>
+    <mergeCell ref="F147:H147"/>
+    <mergeCell ref="F148:H148"/>
+    <mergeCell ref="F149:H149"/>
+    <mergeCell ref="F150:H150"/>
+    <mergeCell ref="F151:H151"/>
+    <mergeCell ref="F152:H152"/>
+    <mergeCell ref="F171:H171"/>
+    <mergeCell ref="F172:H172"/>
+    <mergeCell ref="F173:G173"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="F174:H174"/>
+    <mergeCell ref="F175:H175"/>
+    <mergeCell ref="F159:H159"/>
+    <mergeCell ref="F160:H160"/>
+    <mergeCell ref="F167:H167"/>
+    <mergeCell ref="F168:H168"/>
+    <mergeCell ref="F169:H169"/>
+    <mergeCell ref="F170:H170"/>
     <mergeCell ref="C182:C183"/>
     <mergeCell ref="D182:D183"/>
     <mergeCell ref="E182:E183"/>
@@ -7993,187 +8080,100 @@
     <mergeCell ref="F179:H179"/>
     <mergeCell ref="F180:H180"/>
     <mergeCell ref="F181:H181"/>
-    <mergeCell ref="F171:H171"/>
-    <mergeCell ref="F172:H172"/>
-    <mergeCell ref="F173:G173"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="F174:H174"/>
-    <mergeCell ref="F175:H175"/>
-    <mergeCell ref="F159:H159"/>
-    <mergeCell ref="F160:H160"/>
-    <mergeCell ref="F167:H167"/>
-    <mergeCell ref="F168:H168"/>
-    <mergeCell ref="F169:H169"/>
-    <mergeCell ref="F170:H170"/>
-    <mergeCell ref="C153:E153"/>
-    <mergeCell ref="F153:H153"/>
-    <mergeCell ref="F154:H154"/>
-    <mergeCell ref="F156:H156"/>
-    <mergeCell ref="F157:H157"/>
-    <mergeCell ref="F158:H158"/>
-    <mergeCell ref="F147:H147"/>
-    <mergeCell ref="F148:H148"/>
-    <mergeCell ref="F149:H149"/>
-    <mergeCell ref="F150:H150"/>
-    <mergeCell ref="F151:H151"/>
-    <mergeCell ref="F152:H152"/>
-    <mergeCell ref="F141:H141"/>
-    <mergeCell ref="F142:G142"/>
-    <mergeCell ref="F143:H143"/>
-    <mergeCell ref="F144:H144"/>
-    <mergeCell ref="F145:H145"/>
-    <mergeCell ref="F146:H146"/>
-    <mergeCell ref="F135:H135"/>
-    <mergeCell ref="F136:H136"/>
-    <mergeCell ref="F137:H137"/>
-    <mergeCell ref="F138:H138"/>
-    <mergeCell ref="F139:H139"/>
-    <mergeCell ref="F140:H140"/>
-    <mergeCell ref="F129:G129"/>
-    <mergeCell ref="F130:H130"/>
-    <mergeCell ref="F131:H131"/>
-    <mergeCell ref="F132:H132"/>
-    <mergeCell ref="F133:H133"/>
-    <mergeCell ref="F134:H134"/>
-    <mergeCell ref="F124:H124"/>
-    <mergeCell ref="C125:E125"/>
-    <mergeCell ref="F125:H125"/>
-    <mergeCell ref="F126:G126"/>
-    <mergeCell ref="F127:H127"/>
-    <mergeCell ref="F128:H128"/>
-    <mergeCell ref="F118:H118"/>
-    <mergeCell ref="F119:H119"/>
-    <mergeCell ref="F120:H120"/>
-    <mergeCell ref="F121:H121"/>
-    <mergeCell ref="F122:H122"/>
-    <mergeCell ref="F123:H123"/>
-    <mergeCell ref="F113:H113"/>
-    <mergeCell ref="F114:H114"/>
-    <mergeCell ref="F115:H115"/>
-    <mergeCell ref="F116:H116"/>
-    <mergeCell ref="C117:E117"/>
-    <mergeCell ref="F117:H117"/>
-    <mergeCell ref="F109:H109"/>
-    <mergeCell ref="F110:H110"/>
-    <mergeCell ref="C111:C112"/>
-    <mergeCell ref="D111:D112"/>
-    <mergeCell ref="E111:E112"/>
-    <mergeCell ref="F111:H111"/>
-    <mergeCell ref="F112:H112"/>
-    <mergeCell ref="F103:H103"/>
-    <mergeCell ref="F104:H104"/>
-    <mergeCell ref="F105:H105"/>
-    <mergeCell ref="F106:H106"/>
-    <mergeCell ref="F107:H107"/>
-    <mergeCell ref="F108:H108"/>
-    <mergeCell ref="F97:H97"/>
-    <mergeCell ref="F98:G98"/>
-    <mergeCell ref="F99:H99"/>
-    <mergeCell ref="F100:H100"/>
-    <mergeCell ref="F101:H101"/>
-    <mergeCell ref="F102:H102"/>
-    <mergeCell ref="F91:G91"/>
-    <mergeCell ref="F92:H92"/>
-    <mergeCell ref="F93:H93"/>
-    <mergeCell ref="F94:H94"/>
-    <mergeCell ref="F95:G95"/>
-    <mergeCell ref="F96:G96"/>
-    <mergeCell ref="F85:G85"/>
-    <mergeCell ref="F86:H86"/>
-    <mergeCell ref="F87:H87"/>
-    <mergeCell ref="F88:H88"/>
-    <mergeCell ref="F89:H89"/>
-    <mergeCell ref="F90:G90"/>
-    <mergeCell ref="F80:H80"/>
-    <mergeCell ref="F81:H81"/>
-    <mergeCell ref="F82:H82"/>
-    <mergeCell ref="F83:H83"/>
-    <mergeCell ref="C84:E84"/>
-    <mergeCell ref="F84:H84"/>
-    <mergeCell ref="F74:H74"/>
-    <mergeCell ref="F75:H75"/>
-    <mergeCell ref="F76:H76"/>
-    <mergeCell ref="F77:H77"/>
-    <mergeCell ref="F78:H78"/>
-    <mergeCell ref="F79:H79"/>
-    <mergeCell ref="F68:H68"/>
-    <mergeCell ref="F69:H69"/>
-    <mergeCell ref="F70:H70"/>
-    <mergeCell ref="F71:G71"/>
-    <mergeCell ref="F72:H72"/>
-    <mergeCell ref="F73:H73"/>
-    <mergeCell ref="F62:H62"/>
-    <mergeCell ref="F63:H63"/>
-    <mergeCell ref="F64:H64"/>
-    <mergeCell ref="F65:H65"/>
-    <mergeCell ref="F66:H66"/>
-    <mergeCell ref="F67:H67"/>
-    <mergeCell ref="F56:H56"/>
-    <mergeCell ref="F57:H57"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="F59:H59"/>
-    <mergeCell ref="F60:H60"/>
-    <mergeCell ref="F61:H61"/>
-    <mergeCell ref="F50:H50"/>
-    <mergeCell ref="F51:H51"/>
-    <mergeCell ref="F52:H52"/>
-    <mergeCell ref="F53:H53"/>
-    <mergeCell ref="F54:H54"/>
-    <mergeCell ref="F55:H55"/>
-    <mergeCell ref="F45:H45"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="F46:H46"/>
-    <mergeCell ref="F47:H47"/>
-    <mergeCell ref="F48:H48"/>
-    <mergeCell ref="F49:H49"/>
-    <mergeCell ref="F39:H39"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="F191:H191"/>
+    <mergeCell ref="F192:H192"/>
+    <mergeCell ref="F193:H193"/>
+    <mergeCell ref="F194:H194"/>
+    <mergeCell ref="F195:H195"/>
+    <mergeCell ref="F196:H196"/>
+    <mergeCell ref="F185:H185"/>
+    <mergeCell ref="F186:H186"/>
+    <mergeCell ref="F187:H187"/>
+    <mergeCell ref="F188:H188"/>
+    <mergeCell ref="F189:H189"/>
+    <mergeCell ref="F190:H190"/>
+    <mergeCell ref="C203:C204"/>
+    <mergeCell ref="D203:D204"/>
+    <mergeCell ref="E203:E204"/>
+    <mergeCell ref="F203:H203"/>
+    <mergeCell ref="F205:H205"/>
+    <mergeCell ref="F206:H206"/>
+    <mergeCell ref="F197:H197"/>
+    <mergeCell ref="F198:H198"/>
+    <mergeCell ref="F199:H199"/>
+    <mergeCell ref="F200:H200"/>
+    <mergeCell ref="F201:H201"/>
+    <mergeCell ref="F202:H202"/>
+    <mergeCell ref="F213:H213"/>
+    <mergeCell ref="F214:H214"/>
+    <mergeCell ref="C215:E215"/>
+    <mergeCell ref="F215:H215"/>
+    <mergeCell ref="F216:H216"/>
+    <mergeCell ref="F217:H217"/>
+    <mergeCell ref="F207:H207"/>
+    <mergeCell ref="F208:H208"/>
+    <mergeCell ref="F209:H209"/>
+    <mergeCell ref="F210:H210"/>
+    <mergeCell ref="F211:H211"/>
+    <mergeCell ref="F212:H212"/>
+    <mergeCell ref="F224:H224"/>
+    <mergeCell ref="F225:H225"/>
+    <mergeCell ref="C226:E226"/>
+    <mergeCell ref="F226:H226"/>
+    <mergeCell ref="F227:H227"/>
+    <mergeCell ref="F228:H228"/>
+    <mergeCell ref="F218:H218"/>
+    <mergeCell ref="F219:H219"/>
+    <mergeCell ref="F220:H220"/>
+    <mergeCell ref="F221:H221"/>
+    <mergeCell ref="F222:H222"/>
+    <mergeCell ref="F223:H223"/>
+    <mergeCell ref="F235:G235"/>
+    <mergeCell ref="F236:H236"/>
+    <mergeCell ref="F237:H237"/>
+    <mergeCell ref="F238:H238"/>
+    <mergeCell ref="A239:H239"/>
+    <mergeCell ref="B240:F240"/>
+    <mergeCell ref="F229:H229"/>
+    <mergeCell ref="F230:H230"/>
+    <mergeCell ref="F231:H231"/>
+    <mergeCell ref="F232:H232"/>
+    <mergeCell ref="F233:H233"/>
+    <mergeCell ref="F234:H234"/>
+    <mergeCell ref="B247:F247"/>
+    <mergeCell ref="B248:F248"/>
+    <mergeCell ref="B249:F249"/>
+    <mergeCell ref="B250:F250"/>
+    <mergeCell ref="B251:F251"/>
+    <mergeCell ref="B252:F252"/>
+    <mergeCell ref="B241:F241"/>
+    <mergeCell ref="B242:F242"/>
+    <mergeCell ref="B243:F243"/>
+    <mergeCell ref="B244:F244"/>
+    <mergeCell ref="B245:F245"/>
+    <mergeCell ref="B246:F246"/>
+    <mergeCell ref="B259:F259"/>
+    <mergeCell ref="B260:F260"/>
+    <mergeCell ref="B261:F261"/>
+    <mergeCell ref="B262:F262"/>
+    <mergeCell ref="B263:F263"/>
+    <mergeCell ref="B264:F264"/>
+    <mergeCell ref="B253:F253"/>
+    <mergeCell ref="B254:F254"/>
+    <mergeCell ref="B255:F255"/>
+    <mergeCell ref="B256:F256"/>
+    <mergeCell ref="B257:F257"/>
+    <mergeCell ref="B258:F258"/>
+    <mergeCell ref="G269:H270"/>
+    <mergeCell ref="B271:F272"/>
+    <mergeCell ref="C273:E273"/>
+    <mergeCell ref="C274:E274"/>
+    <mergeCell ref="B265:F265"/>
+    <mergeCell ref="B266:F266"/>
+    <mergeCell ref="B267:F267"/>
+    <mergeCell ref="B268:F268"/>
+    <mergeCell ref="A269:A270"/>
+    <mergeCell ref="B269:F270"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>